<commit_message>
Formula changed according to Catriona
</commit_message>
<xml_diff>
--- a/Outputs/Summary/Nutrients_Transplants_data.xlsx
+++ b/Outputs/Summary/Nutrients_Transplants_data.xlsx
@@ -198,7 +198,7 @@
         <v>30</v>
       </c>
       <c r="E2" t="n">
-        <v>1.5533500000000005</v>
+        <v>-1.9215500000000003</v>
       </c>
     </row>
     <row r="3">
@@ -215,7 +215,7 @@
         <v>30</v>
       </c>
       <c r="E3" t="n">
-        <v>1.13165</v>
+        <v>-1.49985</v>
       </c>
     </row>
     <row r="4">
@@ -232,7 +232,7 @@
         <v>30</v>
       </c>
       <c r="E4" t="n">
-        <v>1.04765</v>
+        <v>-1.4158499999999998</v>
       </c>
     </row>
     <row r="5">
@@ -249,7 +249,7 @@
         <v>30</v>
       </c>
       <c r="E5" t="n">
-        <v>2.2770500000000005</v>
+        <v>-2.6452500000000003</v>
       </c>
     </row>
     <row r="6">
@@ -266,7 +266,7 @@
         <v>30</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7015500000000001</v>
+        <v>-1.06975</v>
       </c>
     </row>
     <row r="7">
@@ -283,7 +283,7 @@
         <v>30</v>
       </c>
       <c r="E7" t="n">
-        <v>1.4583500000000003</v>
+        <v>-1.8265500000000001</v>
       </c>
     </row>
     <row r="8">
@@ -300,7 +300,7 @@
         <v>30</v>
       </c>
       <c r="E8" t="n">
-        <v>0.25129999999999986</v>
+        <v>-1.8429499999999999</v>
       </c>
     </row>
     <row r="9">
@@ -317,7 +317,7 @@
         <v>30</v>
       </c>
       <c r="E9" t="n">
-        <v>0.4966999999999999</v>
+        <v>-2.08835</v>
       </c>
     </row>
     <row r="10">
@@ -334,7 +334,7 @@
         <v>30</v>
       </c>
       <c r="E10" t="n">
-        <v>0.05339999999999989</v>
+        <v>-1.64505</v>
       </c>
     </row>
     <row r="11">
@@ -351,7 +351,7 @@
         <v>30</v>
       </c>
       <c r="E11" t="n">
-        <v>0.6255</v>
+        <v>-2.21715</v>
       </c>
     </row>
     <row r="12">
@@ -368,7 +368,7 @@
         <v>30</v>
       </c>
       <c r="E12" t="n">
-        <v>0.7095</v>
+        <v>-2.30115</v>
       </c>
     </row>
     <row r="13">
@@ -385,7 +385,7 @@
         <v>30</v>
       </c>
       <c r="E13" t="n">
-        <v>1.6932000000000003</v>
+        <v>-3.2848500000000005</v>
       </c>
     </row>
     <row r="14">
@@ -402,7 +402,7 @@
         <v>30</v>
       </c>
       <c r="E14" t="n">
-        <v>3.2274000000000003</v>
+        <v>-4.67065</v>
       </c>
     </row>
     <row r="15">
@@ -419,7 +419,7 @@
         <v>30</v>
       </c>
       <c r="E15" t="n">
-        <v>0.39690000000000003</v>
+        <v>-1.8401500000000002</v>
       </c>
     </row>
     <row r="16">
@@ -436,7 +436,7 @@
         <v>30</v>
       </c>
       <c r="E16" t="n">
-        <v>0.8168000000000002</v>
+        <v>-2.2600500000000006</v>
       </c>
     </row>
     <row r="17">
@@ -453,7 +453,7 @@
         <v>30</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.27990000000000004</v>
+        <v>-1.16335</v>
       </c>
     </row>
     <row r="18">
@@ -470,7 +470,7 @@
         <v>30</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.2794000000000001</v>
+        <v>-1.16385</v>
       </c>
     </row>
     <row r="19">
@@ -487,7 +487,7 @@
         <v>30</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.09699999999999998</v>
+        <v>-1.3462500000000002</v>
       </c>
     </row>
     <row r="20">
@@ -504,7 +504,7 @@
         <v>30</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.3186</v>
+        <v>-6.69665</v>
       </c>
     </row>
     <row r="21">
@@ -521,7 +521,7 @@
         <v>30</v>
       </c>
       <c r="E21" t="n">
-        <v>2.4025999999999996</v>
+        <v>-9.41785</v>
       </c>
     </row>
     <row r="22">
@@ -538,7 +538,7 @@
         <v>30</v>
       </c>
       <c r="E22" t="n">
-        <v>2.2944000000000004</v>
+        <v>-9.309650000000001</v>
       </c>
     </row>
     <row r="23">
@@ -555,7 +555,7 @@
         <v>30</v>
       </c>
       <c r="E23" t="n">
-        <v>-1.1107999999999998</v>
+        <v>-5.904450000000001</v>
       </c>
     </row>
     <row r="24">
@@ -572,7 +572,7 @@
         <v>30</v>
       </c>
       <c r="E24" t="n">
-        <v>1.1178999999999997</v>
+        <v>-8.13315</v>
       </c>
     </row>
     <row r="25">
@@ -589,7 +589,7 @@
         <v>30</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.6991</v>
+        <v>-6.31615</v>
       </c>
     </row>
     <row r="26">
@@ -606,7 +606,7 @@
         <v>30</v>
       </c>
       <c r="E26" t="n">
-        <v>-0.03964999999999996</v>
+        <v>-2.9463999999999997</v>
       </c>
     </row>
     <row r="27">
@@ -623,7 +623,7 @@
         <v>30</v>
       </c>
       <c r="E27" t="n">
-        <v>0.4972500000000002</v>
+        <v>-3.4833</v>
       </c>
     </row>
     <row r="28">
@@ -640,7 +640,7 @@
         <v>30</v>
       </c>
       <c r="E28" t="n">
-        <v>0.7120500000000001</v>
+        <v>-3.6980999999999997</v>
       </c>
     </row>
     <row r="29">
@@ -657,7 +657,7 @@
         <v>30</v>
       </c>
       <c r="E29" t="n">
-        <v>1.57885</v>
+        <v>-4.5649</v>
       </c>
     </row>
     <row r="30">
@@ -674,7 +674,7 @@
         <v>30</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.07545000000000002</v>
+        <v>-2.9105999999999996</v>
       </c>
     </row>
     <row r="31">
@@ -691,7 +691,7 @@
         <v>30</v>
       </c>
       <c r="E31" t="n">
-        <v>1.4520500000000007</v>
+        <v>-4.4381</v>
       </c>
     </row>
     <row r="32">
@@ -708,7 +708,7 @@
         <v>30</v>
       </c>
       <c r="E32" t="n">
-        <v>-0.14884999999999993</v>
+        <v>-2.2845500000000003</v>
       </c>
     </row>
     <row r="33">
@@ -725,7 +725,7 @@
         <v>30</v>
       </c>
       <c r="E33" t="n">
-        <v>-0.5764500000000001</v>
+        <v>-1.85695</v>
       </c>
     </row>
     <row r="34">
@@ -742,7 +742,7 @@
         <v>30</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.4577500000000001</v>
+        <v>-1.9756500000000001</v>
       </c>
     </row>
     <row r="35">
@@ -759,7 +759,7 @@
         <v>30</v>
       </c>
       <c r="E35" t="n">
-        <v>-0.6725500000000002</v>
+        <v>-1.76085</v>
       </c>
     </row>
     <row r="36">
@@ -776,7 +776,7 @@
         <v>30</v>
       </c>
       <c r="E36" t="n">
-        <v>-0.5783500000000001</v>
+        <v>-1.85505</v>
       </c>
     </row>
     <row r="37">
@@ -793,7 +793,7 @@
         <v>30</v>
       </c>
       <c r="E37" t="n">
-        <v>-0.40605000000000024</v>
+        <v>-2.02735</v>
       </c>
     </row>
     <row r="38">
@@ -810,7 +810,7 @@
         <v>30</v>
       </c>
       <c r="E38" t="n">
-        <v>4.38115</v>
+        <v>-5.883450000000001</v>
       </c>
     </row>
     <row r="39">
@@ -827,7 +827,7 @@
         <v>30</v>
       </c>
       <c r="E39" t="n">
-        <v>0.045949999999999935</v>
+        <v>-1.5482500000000008</v>
       </c>
     </row>
     <row r="40">
@@ -844,7 +844,7 @@
         <v>30</v>
       </c>
       <c r="E40" t="n">
-        <v>4.078749999999999</v>
+        <v>-5.58105</v>
       </c>
     </row>
     <row r="41">
@@ -861,7 +861,7 @@
         <v>30</v>
       </c>
       <c r="E41" t="n">
-        <v>3.2047499999999998</v>
+        <v>-4.707050000000001</v>
       </c>
     </row>
     <row r="42">
@@ -878,7 +878,7 @@
         <v>30</v>
       </c>
       <c r="E42" t="n">
-        <v>-1.01635</v>
+        <v>-0.48595000000000077</v>
       </c>
     </row>
     <row r="43">
@@ -895,7 +895,7 @@
         <v>30</v>
       </c>
       <c r="E43" t="n">
-        <v>0.3773499999999994</v>
+        <v>-1.8796500000000003</v>
       </c>
     </row>
     <row r="44">
@@ -912,7 +912,7 @@
         <v>30</v>
       </c>
       <c r="E44" t="n">
-        <v>-1.18845</v>
+        <v>-0.3503000000000003</v>
       </c>
     </row>
     <row r="45">
@@ -929,7 +929,7 @@
         <v>30</v>
       </c>
       <c r="E45" t="n">
-        <v>2.6647499999999997</v>
+        <v>-4.2035</v>
       </c>
     </row>
     <row r="46">
@@ -946,7 +946,7 @@
         <v>30</v>
       </c>
       <c r="E46" t="n">
-        <v>-0.07874999999999988</v>
+        <v>-1.4600000000000004</v>
       </c>
     </row>
     <row r="47">
@@ -963,7 +963,7 @@
         <v>30</v>
       </c>
       <c r="E47" t="n">
-        <v>2.4898499999999997</v>
+        <v>-4.0286</v>
       </c>
     </row>
     <row r="48">
@@ -980,7 +980,7 @@
         <v>30</v>
       </c>
       <c r="E48" t="n">
-        <v>-0.5924499999999999</v>
+        <v>-0.9463000000000004</v>
       </c>
     </row>
     <row r="49">
@@ -997,7 +997,7 @@
         <v>30</v>
       </c>
       <c r="E49" t="n">
-        <v>-1.56705</v>
+        <v>0.02829999999999977</v>
       </c>
     </row>
     <row r="50">
@@ -1014,7 +1014,7 @@
         <v>30</v>
       </c>
       <c r="E50" t="n">
-        <v>-0.5600499999999999</v>
+        <v>0.15700000000000047</v>
       </c>
     </row>
     <row r="51">
@@ -1031,7 +1031,7 @@
         <v>30</v>
       </c>
       <c r="E51" t="n">
-        <v>-0.41934999999999967</v>
+        <v>0.016300000000000203</v>
       </c>
     </row>
     <row r="52">
@@ -1048,7 +1048,7 @@
         <v>30</v>
       </c>
       <c r="E52" t="n">
-        <v>-1.3169499999999998</v>
+        <v>0.9139000000000004</v>
       </c>
     </row>
     <row r="53">
@@ -1065,7 +1065,7 @@
         <v>30</v>
       </c>
       <c r="E53" t="n">
-        <v>1.9981500000000003</v>
+        <v>-2.4012</v>
       </c>
     </row>
     <row r="54">
@@ -1082,7 +1082,7 @@
         <v>30</v>
       </c>
       <c r="E54" t="n">
-        <v>0.06505000000000027</v>
+        <v>-0.46809999999999974</v>
       </c>
     </row>
     <row r="55">
@@ -1099,7 +1099,7 @@
         <v>30</v>
       </c>
       <c r="E55" t="n">
-        <v>-0.5286499999999998</v>
+        <v>0.12560000000000038</v>
       </c>
     </row>
     <row r="56">
@@ -1116,7 +1116,7 @@
         <v>30</v>
       </c>
       <c r="E56" t="n">
-        <v>-0.4979500000000001</v>
+        <v>-0.19430000000000014</v>
       </c>
     </row>
     <row r="57">
@@ -1133,7 +1133,7 @@
         <v>30</v>
       </c>
       <c r="E57" t="n">
-        <v>0.06474999999999986</v>
+        <v>-0.7570000000000001</v>
       </c>
     </row>
     <row r="58">
@@ -1150,7 +1150,7 @@
         <v>30</v>
       </c>
       <c r="E58" t="n">
-        <v>-0.55595</v>
+        <v>-0.1363000000000002</v>
       </c>
     </row>
     <row r="59">
@@ -1167,7 +1167,7 @@
         <v>30</v>
       </c>
       <c r="E59" t="n">
-        <v>-0.08225000000000005</v>
+        <v>-0.6100000000000002</v>
       </c>
     </row>
     <row r="60">
@@ -1184,7 +1184,7 @@
         <v>30</v>
       </c>
       <c r="E60" t="n">
-        <v>1.45605</v>
+        <v>-2.1483000000000003</v>
       </c>
     </row>
     <row r="61">
@@ -1201,7 +1201,7 @@
         <v>30</v>
       </c>
       <c r="E61" t="n">
-        <v>0.5586499999999999</v>
+        <v>-1.2509000000000001</v>
       </c>
     </row>
     <row r="62">
@@ -1218,7 +1218,7 @@
         <v>30</v>
       </c>
       <c r="E62" t="n">
-        <v>3.994849999999999</v>
+        <v>-7.175199999999999</v>
       </c>
     </row>
     <row r="63">
@@ -1235,7 +1235,7 @@
         <v>30</v>
       </c>
       <c r="E63" t="n">
-        <v>-0.29295000000000004</v>
+        <v>-2.8874000000000004</v>
       </c>
     </row>
     <row r="64">
@@ -1252,7 +1252,7 @@
         <v>30</v>
       </c>
       <c r="E64" t="n">
-        <v>-1.27795</v>
+        <v>-1.9024000000000003</v>
       </c>
     </row>
     <row r="65">
@@ -1269,7 +1269,7 @@
         <v>30</v>
       </c>
       <c r="E65" t="n">
-        <v>-1.3470499999999999</v>
+        <v>-1.8333000000000004</v>
       </c>
     </row>
     <row r="66">
@@ -1286,7 +1286,7 @@
         <v>30</v>
       </c>
       <c r="E66" t="n">
-        <v>-1.21655</v>
+        <v>-1.9638000000000002</v>
       </c>
     </row>
     <row r="67">
@@ -1303,7 +1303,7 @@
         <v>30</v>
       </c>
       <c r="E67" t="n">
-        <v>-1.62215</v>
+        <v>-1.5582000000000003</v>
       </c>
     </row>
     <row r="68">
@@ -1320,7 +1320,7 @@
         <v>30</v>
       </c>
       <c r="E68" t="n">
-        <v>-1.1282999999999999</v>
+        <v>0.23665000000000003</v>
       </c>
     </row>
     <row r="69">
@@ -1337,7 +1337,7 @@
         <v>30</v>
       </c>
       <c r="E69" t="n">
-        <v>-1.1678</v>
+        <v>0.2761500000000001</v>
       </c>
     </row>
     <row r="70">
@@ -1354,7 +1354,7 @@
         <v>30</v>
       </c>
       <c r="E70" t="n">
-        <v>-1.5485999999999998</v>
+        <v>0.6569499999999999</v>
       </c>
     </row>
     <row r="71">
@@ -1371,7 +1371,7 @@
         <v>30</v>
       </c>
       <c r="E71" t="n">
-        <v>-1.0027</v>
+        <v>0.1110500000000001</v>
       </c>
     </row>
     <row r="72">
@@ -1388,7 +1388,7 @@
         <v>30</v>
       </c>
       <c r="E72" t="n">
-        <v>-0.32299999999999995</v>
+        <v>-0.5686499999999999</v>
       </c>
     </row>
     <row r="73">
@@ -1405,7 +1405,7 @@
         <v>30</v>
       </c>
       <c r="E73" t="n">
-        <v>-1.0675999999999999</v>
+        <v>0.17595000000000005</v>
       </c>
     </row>
     <row r="74">
@@ -1422,7 +1422,7 @@
         <v>31</v>
       </c>
       <c r="E74" t="n">
-        <v>0.0904</v>
+        <v>-0.09749999999999999</v>
       </c>
     </row>
     <row r="75">
@@ -1439,7 +1439,7 @@
         <v>31</v>
       </c>
       <c r="E75" t="n">
-        <v>0.0878</v>
+        <v>-0.0949</v>
       </c>
     </row>
     <row r="76">
@@ -1456,7 +1456,7 @@
         <v>31</v>
       </c>
       <c r="E76" t="n">
-        <v>0.3328</v>
+        <v>-0.3399</v>
       </c>
     </row>
     <row r="77">
@@ -1473,7 +1473,7 @@
         <v>31</v>
       </c>
       <c r="E77" t="n">
-        <v>0.16960000000000003</v>
+        <v>-0.17670000000000002</v>
       </c>
     </row>
     <row r="78">
@@ -1490,7 +1490,7 @@
         <v>31</v>
       </c>
       <c r="E78" t="n">
-        <v>0.19190000000000002</v>
+        <v>-0.199</v>
       </c>
     </row>
     <row r="79">
@@ -1507,7 +1507,7 @@
         <v>31</v>
       </c>
       <c r="E79" t="n">
-        <v>0.2373</v>
+        <v>-0.2444</v>
       </c>
     </row>
     <row r="80">
@@ -1524,7 +1524,7 @@
         <v>31</v>
       </c>
       <c r="E80" t="n">
-        <v>-0.010749999999999982</v>
+        <v>-0.20125</v>
       </c>
     </row>
     <row r="81">
@@ -1541,7 +1541,7 @@
         <v>31</v>
       </c>
       <c r="E81" t="n">
-        <v>0.006950000000000012</v>
+        <v>-0.21895</v>
       </c>
     </row>
     <row r="82">
@@ -1558,7 +1558,7 @@
         <v>31</v>
       </c>
       <c r="E82" t="n">
-        <v>-0.04434999999999999</v>
+        <v>-0.16765000000000002</v>
       </c>
     </row>
     <row r="83">
@@ -1575,7 +1575,7 @@
         <v>31</v>
       </c>
       <c r="E83" t="n">
-        <v>0.20854999999999999</v>
+        <v>-0.42055</v>
       </c>
     </row>
     <row r="84">
@@ -1592,7 +1592,7 @@
         <v>31</v>
       </c>
       <c r="E84" t="n">
-        <v>-0.024249999999999994</v>
+        <v>-0.18775</v>
       </c>
     </row>
     <row r="85">
@@ -1609,7 +1609,7 @@
         <v>31</v>
       </c>
       <c r="E85" t="n">
-        <v>0.04965</v>
+        <v>-0.26165</v>
       </c>
     </row>
     <row r="86">
@@ -1626,7 +1626,7 @@
         <v>31</v>
       </c>
       <c r="E86" t="n">
-        <v>0.016149999999999998</v>
+        <v>-0.18030000000000002</v>
       </c>
     </row>
     <row r="87">
@@ -1643,7 +1643,7 @@
         <v>31</v>
       </c>
       <c r="E87" t="n">
-        <v>-0.004250000000000004</v>
+        <v>-0.15990000000000001</v>
       </c>
     </row>
     <row r="88">
@@ -1660,7 +1660,7 @@
         <v>31</v>
       </c>
       <c r="E88" t="n">
-        <v>0.031549999999999995</v>
+        <v>-0.1957</v>
       </c>
     </row>
     <row r="89">
@@ -1677,7 +1677,7 @@
         <v>31</v>
       </c>
       <c r="E89" t="n">
-        <v>-0.036150000000000015</v>
+        <v>-0.128</v>
       </c>
     </row>
     <row r="90">
@@ -1694,7 +1694,7 @@
         <v>31</v>
       </c>
       <c r="E90" t="n">
-        <v>-0.07905000000000001</v>
+        <v>-0.08510000000000001</v>
       </c>
     </row>
     <row r="91">
@@ -1711,7 +1711,7 @@
         <v>31</v>
       </c>
       <c r="E91" t="n">
-        <v>-0.05145000000000001</v>
+        <v>-0.11270000000000001</v>
       </c>
     </row>
     <row r="92">
@@ -1728,7 +1728,7 @@
         <v>31</v>
       </c>
       <c r="E92" t="n">
-        <v>0.13490000000000002</v>
+        <v>-0.43234999999999996</v>
       </c>
     </row>
     <row r="93">
@@ -1745,7 +1745,7 @@
         <v>31</v>
       </c>
       <c r="E93" t="n">
-        <v>0.01160000000000004</v>
+        <v>-0.30905</v>
       </c>
     </row>
     <row r="94">
@@ -1762,7 +1762,7 @@
         <v>31</v>
       </c>
       <c r="E94" t="n">
-        <v>0.48390000000000016</v>
+        <v>-0.7813500000000001</v>
       </c>
     </row>
     <row r="95">
@@ -1779,7 +1779,7 @@
         <v>31</v>
       </c>
       <c r="E95" t="n">
-        <v>-0.04969999999999998</v>
+        <v>-0.24774999999999997</v>
       </c>
     </row>
     <row r="96">
@@ -1796,7 +1796,7 @@
         <v>31</v>
       </c>
       <c r="E96" t="n">
-        <v>0.0030000000000000443</v>
+        <v>-0.30045</v>
       </c>
     </row>
     <row r="97">
@@ -1813,7 +1813,7 @@
         <v>31</v>
       </c>
       <c r="E97" t="n">
-        <v>-0.048399999999999985</v>
+        <v>-0.24904999999999997</v>
       </c>
     </row>
     <row r="98">
@@ -1830,7 +1830,7 @@
         <v>31</v>
       </c>
       <c r="E98" t="n">
-        <v>0.06334999999999999</v>
+        <v>-0.09784999999999999</v>
       </c>
     </row>
     <row r="99">
@@ -1847,7 +1847,7 @@
         <v>31</v>
       </c>
       <c r="E99" t="n">
-        <v>0.07855</v>
+        <v>-0.11305</v>
       </c>
     </row>
     <row r="100">
@@ -1864,7 +1864,7 @@
         <v>31</v>
       </c>
       <c r="E100" t="n">
-        <v>0.07554999999999999</v>
+        <v>-0.11005</v>
       </c>
     </row>
     <row r="101">
@@ -1881,7 +1881,7 @@
         <v>31</v>
       </c>
       <c r="E101" t="n">
-        <v>0.09005</v>
+        <v>-0.12455000000000001</v>
       </c>
     </row>
     <row r="102">
@@ -1898,7 +1898,7 @@
         <v>31</v>
       </c>
       <c r="E102" t="n">
-        <v>0.05685</v>
+        <v>-0.09135</v>
       </c>
     </row>
     <row r="103">
@@ -1915,7 +1915,7 @@
         <v>31</v>
       </c>
       <c r="E103" t="n">
-        <v>0.07315</v>
+        <v>-0.10765000000000001</v>
       </c>
     </row>
     <row r="104">
@@ -1932,7 +1932,7 @@
         <v>31</v>
       </c>
       <c r="E104" t="n">
-        <v>0.0179</v>
+        <v>-0.0852</v>
       </c>
     </row>
     <row r="105">
@@ -1949,7 +1949,7 @@
         <v>31</v>
       </c>
       <c r="E105" t="n">
-        <v>-0.024799999999999996</v>
+        <v>-0.0425</v>
       </c>
     </row>
     <row r="106">
@@ -1966,7 +1966,7 @@
         <v>31</v>
       </c>
       <c r="E106" t="n">
-        <v>0.0469</v>
+        <v>-0.1142</v>
       </c>
     </row>
     <row r="107">
@@ -1983,7 +1983,7 @@
         <v>31</v>
       </c>
       <c r="E107" t="n">
-        <v>-0.02679999999999999</v>
+        <v>-0.04050000000000001</v>
       </c>
     </row>
     <row r="108">
@@ -2000,7 +2000,7 @@
         <v>31</v>
       </c>
       <c r="E108" t="n">
-        <v>0.016600000000000004</v>
+        <v>-0.0839</v>
       </c>
     </row>
     <row r="109">
@@ -2017,7 +2017,7 @@
         <v>31</v>
       </c>
       <c r="E109" t="n">
-        <v>0.045</v>
+        <v>-0.1123</v>
       </c>
     </row>
     <row r="110">
@@ -2034,7 +2034,7 @@
         <v>31</v>
       </c>
       <c r="E110" t="n">
-        <v>0.14959999999999996</v>
+        <v>-0.33085</v>
       </c>
     </row>
     <row r="111">
@@ -2051,7 +2051,7 @@
         <v>31</v>
       </c>
       <c r="E111" t="n">
-        <v>-0.0714</v>
+        <v>-0.10984999999999999</v>
       </c>
     </row>
     <row r="112">
@@ -2068,7 +2068,7 @@
         <v>31</v>
       </c>
       <c r="E112" t="n">
-        <v>-0.02260000000000001</v>
+        <v>-0.15864999999999999</v>
       </c>
     </row>
     <row r="113">
@@ -2085,7 +2085,7 @@
         <v>31</v>
       </c>
       <c r="E113" t="n">
-        <v>0.172</v>
+        <v>-0.35324999999999995</v>
       </c>
     </row>
     <row r="114">
@@ -2102,7 +2102,7 @@
         <v>31</v>
       </c>
       <c r="E114" t="n">
-        <v>-0.017000000000000015</v>
+        <v>-0.16424999999999998</v>
       </c>
     </row>
     <row r="115">
@@ -2119,7 +2119,7 @@
         <v>31</v>
       </c>
       <c r="E115" t="n">
-        <v>0.06409999999999999</v>
+        <v>-0.24534999999999998</v>
       </c>
     </row>
     <row r="116">
@@ -2136,7 +2136,7 @@
         <v>31</v>
       </c>
       <c r="E116" t="n">
-        <v>0.07244999999999999</v>
+        <v>-0.022649999999999976</v>
       </c>
     </row>
     <row r="117">
@@ -2153,7 +2153,7 @@
         <v>31</v>
       </c>
       <c r="E117" t="n">
-        <v>0.08365</v>
+        <v>-0.03384999999999999</v>
       </c>
     </row>
     <row r="118">
@@ -2170,7 +2170,7 @@
         <v>31</v>
       </c>
       <c r="E118" t="n">
-        <v>0.12705000000000002</v>
+        <v>-0.07725000000000001</v>
       </c>
     </row>
     <row r="119">
@@ -2187,7 +2187,7 @@
         <v>31</v>
       </c>
       <c r="E119" t="n">
-        <v>0.08325000000000002</v>
+        <v>-0.03345000000000001</v>
       </c>
     </row>
     <row r="120">
@@ -2204,7 +2204,7 @@
         <v>31</v>
       </c>
       <c r="E120" t="n">
-        <v>0.15464999999999998</v>
+        <v>-0.10484999999999997</v>
       </c>
     </row>
     <row r="121">
@@ -2221,7 +2221,7 @@
         <v>31</v>
       </c>
       <c r="E121" t="n">
-        <v>0.024349999999999997</v>
+        <v>0.025450000000000014</v>
       </c>
     </row>
     <row r="122">
@@ -2238,7 +2238,7 @@
         <v>31</v>
       </c>
       <c r="E122" t="n">
-        <v>-0.03555</v>
+        <v>-0.12284999999999999</v>
       </c>
     </row>
     <row r="123">
@@ -2255,7 +2255,7 @@
         <v>31</v>
       </c>
       <c r="E123" t="n">
-        <v>0.10644999999999999</v>
+        <v>-0.26485</v>
       </c>
     </row>
     <row r="124">
@@ -2272,7 +2272,7 @@
         <v>31</v>
       </c>
       <c r="E124" t="n">
-        <v>0.005650000000000016</v>
+        <v>-0.16405</v>
       </c>
     </row>
     <row r="125">
@@ -2289,7 +2289,7 @@
         <v>31</v>
       </c>
       <c r="E125" t="n">
-        <v>-0.03075</v>
+        <v>-0.12764999999999999</v>
       </c>
     </row>
     <row r="126">
@@ -2306,7 +2306,7 @@
         <v>31</v>
       </c>
       <c r="E126" t="n">
-        <v>0.07175000000000004</v>
+        <v>-0.23015000000000002</v>
       </c>
     </row>
     <row r="127">
@@ -2323,7 +2323,7 @@
         <v>31</v>
       </c>
       <c r="E127" t="n">
-        <v>0.009649999999999992</v>
+        <v>-0.16804999999999998</v>
       </c>
     </row>
     <row r="128">
@@ -2340,7 +2340,7 @@
         <v>31</v>
       </c>
       <c r="E128" t="n">
-        <v>-0.016200000000000006</v>
+        <v>-0.029849999999999974</v>
       </c>
     </row>
     <row r="129">
@@ -2357,7 +2357,7 @@
         <v>31</v>
       </c>
       <c r="E129" t="n">
-        <v>0.03270000000000001</v>
+        <v>-0.07874999999999999</v>
       </c>
     </row>
     <row r="130">
@@ -2374,7 +2374,7 @@
         <v>31</v>
       </c>
       <c r="E130" t="n">
-        <v>-0.03960000000000001</v>
+        <v>-0.00644999999999997</v>
       </c>
     </row>
     <row r="131">
@@ -2391,7 +2391,7 @@
         <v>31</v>
       </c>
       <c r="E131" t="n">
-        <v>0.02980000000000002</v>
+        <v>-0.07585</v>
       </c>
     </row>
     <row r="132">
@@ -2408,7 +2408,7 @@
         <v>31</v>
       </c>
       <c r="E132" t="n">
-        <v>-0.01100000000000001</v>
+        <v>-0.03504999999999997</v>
       </c>
     </row>
     <row r="133">
@@ -2425,7 +2425,7 @@
         <v>31</v>
       </c>
       <c r="E133" t="n">
-        <v>-0.02310000000000001</v>
+        <v>-0.02294999999999997</v>
       </c>
     </row>
     <row r="134">
@@ -2442,7 +2442,7 @@
         <v>31</v>
       </c>
       <c r="E134" t="n">
-        <v>0.06640000000000001</v>
+        <v>-0.1891</v>
       </c>
     </row>
     <row r="135">
@@ -2459,7 +2459,7 @@
         <v>31</v>
       </c>
       <c r="E135" t="n">
-        <v>0.07590000000000002</v>
+        <v>-0.1986</v>
       </c>
     </row>
     <row r="136">
@@ -2476,7 +2476,7 @@
         <v>31</v>
       </c>
       <c r="E136" t="n">
-        <v>0.004299999999999998</v>
+        <v>-0.127</v>
       </c>
     </row>
     <row r="137">
@@ -2493,7 +2493,7 @@
         <v>31</v>
       </c>
       <c r="E137" t="n">
-        <v>-0.0384</v>
+        <v>-0.08429999999999999</v>
       </c>
     </row>
     <row r="138">
@@ -2510,7 +2510,7 @@
         <v>31</v>
       </c>
       <c r="E138" t="n">
-        <v>0.0655</v>
+        <v>-0.18819999999999998</v>
       </c>
     </row>
     <row r="139">
@@ -2527,7 +2527,7 @@
         <v>31</v>
       </c>
       <c r="E139" t="n">
-        <v>-0.0392</v>
+        <v>-0.08349999999999999</v>
       </c>
     </row>
     <row r="140">
@@ -2544,7 +2544,7 @@
         <v>31</v>
       </c>
       <c r="E140" t="n">
-        <v>-0.13145000000000004</v>
+        <v>-0.19725</v>
       </c>
     </row>
     <row r="141">
@@ -2561,7 +2561,7 @@
         <v>31</v>
       </c>
       <c r="E141" t="n">
-        <v>-0.17475000000000002</v>
+        <v>-0.15395000000000003</v>
       </c>
     </row>
     <row r="142">
@@ -2595,7 +2595,7 @@
         <v>31</v>
       </c>
       <c r="E143" t="n">
-        <v>-0.16375000000000003</v>
+        <v>-0.16495</v>
       </c>
     </row>
     <row r="144">
@@ -2612,7 +2612,7 @@
         <v>31</v>
       </c>
       <c r="E144" t="n">
-        <v>-0.14235000000000003</v>
+        <v>-0.18635000000000002</v>
       </c>
     </row>
     <row r="145">
@@ -2629,7 +2629,7 @@
         <v>31</v>
       </c>
       <c r="E145" t="n">
-        <v>-0.17955000000000004</v>
+        <v>-0.14915</v>
       </c>
     </row>
     <row r="146">
@@ -2646,7 +2646,7 @@
         <v>32</v>
       </c>
       <c r="E146" t="n">
-        <v>0.0479</v>
+        <v>-0.08345</v>
       </c>
     </row>
     <row r="147">
@@ -2663,7 +2663,7 @@
         <v>32</v>
       </c>
       <c r="E147" t="n">
-        <v>0.10890000000000001</v>
+        <v>-0.14445000000000002</v>
       </c>
     </row>
     <row r="148">
@@ -2680,7 +2680,7 @@
         <v>32</v>
       </c>
       <c r="E148" t="n">
-        <v>0.08270000000000001</v>
+        <v>-0.11825000000000001</v>
       </c>
     </row>
     <row r="149">
@@ -2697,7 +2697,7 @@
         <v>32</v>
       </c>
       <c r="E149" t="n">
-        <v>0.13119999999999998</v>
+        <v>-0.16675</v>
       </c>
     </row>
     <row r="150">
@@ -2714,7 +2714,7 @@
         <v>32</v>
       </c>
       <c r="E150" t="n">
-        <v>0.06530000000000001</v>
+        <v>-0.10085000000000001</v>
       </c>
     </row>
     <row r="151">
@@ -2731,7 +2731,7 @@
         <v>32</v>
       </c>
       <c r="E151" t="n">
-        <v>0.07939999999999998</v>
+        <v>-0.11494999999999998</v>
       </c>
     </row>
     <row r="152">
@@ -2748,7 +2748,7 @@
         <v>32</v>
       </c>
       <c r="E152" t="n">
-        <v>0.015700000000000006</v>
+        <v>-0.08949999999999998</v>
       </c>
     </row>
     <row r="153">
@@ -2765,7 +2765,7 @@
         <v>32</v>
       </c>
       <c r="E153" t="n">
-        <v>0.05449999999999999</v>
+        <v>-0.12829999999999997</v>
       </c>
     </row>
     <row r="154">
@@ -2782,7 +2782,7 @@
         <v>32</v>
       </c>
       <c r="E154" t="n">
-        <v>0.025400000000000006</v>
+        <v>-0.09919999999999998</v>
       </c>
     </row>
     <row r="155">
@@ -2799,7 +2799,7 @@
         <v>32</v>
       </c>
       <c r="E155" t="n">
-        <v>0.048100000000000004</v>
+        <v>-0.12189999999999998</v>
       </c>
     </row>
     <row r="156">
@@ -2816,7 +2816,7 @@
         <v>32</v>
       </c>
       <c r="E156" t="n">
-        <v>0.029500000000000026</v>
+        <v>-0.1033</v>
       </c>
     </row>
     <row r="157">
@@ -2833,7 +2833,7 @@
         <v>32</v>
       </c>
       <c r="E157" t="n">
-        <v>0.09820000000000001</v>
+        <v>-0.172</v>
       </c>
     </row>
     <row r="158">
@@ -2850,7 +2850,7 @@
         <v>32</v>
       </c>
       <c r="E158" t="n">
-        <v>0.07884999999999999</v>
+        <v>-0.1508</v>
       </c>
     </row>
     <row r="159">
@@ -2867,7 +2867,7 @@
         <v>32</v>
       </c>
       <c r="E159" t="n">
-        <v>0.04445</v>
+        <v>-0.11639999999999999</v>
       </c>
     </row>
     <row r="160">
@@ -2884,7 +2884,7 @@
         <v>32</v>
       </c>
       <c r="E160" t="n">
-        <v>0.05135000000000001</v>
+        <v>-0.12329999999999999</v>
       </c>
     </row>
     <row r="161">
@@ -2901,7 +2901,7 @@
         <v>32</v>
       </c>
       <c r="E161" t="n">
-        <v>0.030750000000000013</v>
+        <v>-0.1027</v>
       </c>
     </row>
     <row r="162">
@@ -2918,7 +2918,7 @@
         <v>32</v>
       </c>
       <c r="E162" t="n">
-        <v>0.012950000000000003</v>
+        <v>-0.08489999999999999</v>
       </c>
     </row>
     <row r="163">
@@ -2935,7 +2935,7 @@
         <v>32</v>
       </c>
       <c r="E163" t="n">
-        <v>0.04605000000000001</v>
+        <v>-0.118</v>
       </c>
     </row>
     <row r="164">
@@ -2952,7 +2952,7 @@
         <v>32</v>
       </c>
       <c r="E164" t="n">
-        <v>0.015199999999999991</v>
+        <v>-0.18239999999999998</v>
       </c>
     </row>
     <row r="165">
@@ -2969,7 +2969,7 @@
         <v>32</v>
       </c>
       <c r="E165" t="n">
-        <v>0.0343</v>
+        <v>-0.20149999999999998</v>
       </c>
     </row>
     <row r="166">
@@ -2986,7 +2986,7 @@
         <v>32</v>
       </c>
       <c r="E166" t="n">
-        <v>0.04869999999999999</v>
+        <v>-0.21589999999999998</v>
       </c>
     </row>
     <row r="167">
@@ -3003,7 +3003,7 @@
         <v>32</v>
       </c>
       <c r="E167" t="n">
-        <v>-0.044399999999999995</v>
+        <v>-0.12279999999999999</v>
       </c>
     </row>
     <row r="168">
@@ -3020,7 +3020,7 @@
         <v>32</v>
       </c>
       <c r="E168" t="n">
-        <v>0.009300000000000003</v>
+        <v>-0.1765</v>
       </c>
     </row>
     <row r="169">
@@ -3037,7 +3037,7 @@
         <v>32</v>
       </c>
       <c r="E169" t="n">
-        <v>-0.016399999999999998</v>
+        <v>-0.1508</v>
       </c>
     </row>
     <row r="170">
@@ -3054,7 +3054,7 @@
         <v>32</v>
       </c>
       <c r="E170" t="n">
-        <v>0.03564999999999999</v>
+        <v>-0.09359999999999999</v>
       </c>
     </row>
     <row r="171">
@@ -3071,7 +3071,7 @@
         <v>32</v>
       </c>
       <c r="E171" t="n">
-        <v>0.05895</v>
+        <v>-0.1169</v>
       </c>
     </row>
     <row r="172">
@@ -3088,7 +3088,7 @@
         <v>32</v>
       </c>
       <c r="E172" t="n">
-        <v>0.07535</v>
+        <v>-0.1333</v>
       </c>
     </row>
     <row r="173">
@@ -3105,7 +3105,7 @@
         <v>32</v>
       </c>
       <c r="E173" t="n">
-        <v>0.05235000000000001</v>
+        <v>-0.11030000000000001</v>
       </c>
     </row>
     <row r="174">
@@ -3122,7 +3122,7 @@
         <v>32</v>
       </c>
       <c r="E174" t="n">
-        <v>0.02005</v>
+        <v>-0.078</v>
       </c>
     </row>
     <row r="175">
@@ -3139,7 +3139,7 @@
         <v>32</v>
       </c>
       <c r="E175" t="n">
-        <v>0.036750000000000005</v>
+        <v>-0.0947</v>
       </c>
     </row>
     <row r="176">
@@ -3156,7 +3156,7 @@
         <v>32</v>
       </c>
       <c r="E176" t="n">
-        <v>0.04970000000000001</v>
+        <v>-0.11059999999999999</v>
       </c>
     </row>
     <row r="177">
@@ -3173,7 +3173,7 @@
         <v>32</v>
       </c>
       <c r="E177" t="n">
-        <v>0.025900000000000006</v>
+        <v>-0.08679999999999999</v>
       </c>
     </row>
     <row r="178">
@@ -3190,7 +3190,7 @@
         <v>32</v>
       </c>
       <c r="E178" t="n">
-        <v>0.0349</v>
+        <v>-0.09579999999999998</v>
       </c>
     </row>
     <row r="179">
@@ -3207,7 +3207,7 @@
         <v>32</v>
       </c>
       <c r="E179" t="n">
-        <v>-0.0024999999999999953</v>
+        <v>-0.05839999999999999</v>
       </c>
     </row>
     <row r="180">
@@ -3224,7 +3224,7 @@
         <v>32</v>
       </c>
       <c r="E180" t="n">
-        <v>0.019299999999999998</v>
+        <v>-0.08019999999999998</v>
       </c>
     </row>
     <row r="181">
@@ -3241,7 +3241,7 @@
         <v>32</v>
       </c>
       <c r="E181" t="n">
-        <v>0.0493</v>
+        <v>-0.11019999999999998</v>
       </c>
     </row>
     <row r="182">
@@ -3258,7 +3258,7 @@
         <v>32</v>
       </c>
       <c r="E182" t="n">
-        <v>0.04844999999999999</v>
+        <v>-0.10975000000000001</v>
       </c>
     </row>
     <row r="183">
@@ -3275,7 +3275,7 @@
         <v>32</v>
       </c>
       <c r="E183" t="n">
-        <v>0.01214999999999998</v>
+        <v>-0.07345</v>
       </c>
     </row>
     <row r="184">
@@ -3292,7 +3292,7 @@
         <v>32</v>
       </c>
       <c r="E184" t="n">
-        <v>0.03624999999999998</v>
+        <v>-0.09755</v>
       </c>
     </row>
     <row r="185">
@@ -3309,7 +3309,7 @@
         <v>32</v>
       </c>
       <c r="E185" t="n">
-        <v>0.06444999999999998</v>
+        <v>-0.12575</v>
       </c>
     </row>
     <row r="186">
@@ -3326,7 +3326,7 @@
         <v>32</v>
       </c>
       <c r="E186" t="n">
-        <v>-0.003050000000000011</v>
+        <v>-0.05825000000000001</v>
       </c>
     </row>
     <row r="187">
@@ -3343,7 +3343,7 @@
         <v>32</v>
       </c>
       <c r="E187" t="n">
-        <v>0.030049999999999993</v>
+        <v>-0.09135000000000001</v>
       </c>
     </row>
     <row r="188">
@@ -3360,7 +3360,7 @@
         <v>32</v>
       </c>
       <c r="E188" t="n">
-        <v>0.020899999999999988</v>
+        <v>-0.0819</v>
       </c>
     </row>
     <row r="189">
@@ -3377,7 +3377,7 @@
         <v>32</v>
       </c>
       <c r="E189" t="n">
-        <v>0.0556</v>
+        <v>-0.11660000000000001</v>
       </c>
     </row>
     <row r="190">
@@ -3394,7 +3394,7 @@
         <v>32</v>
       </c>
       <c r="E190" t="n">
-        <v>0.014299999999999993</v>
+        <v>-0.0753</v>
       </c>
     </row>
     <row r="191">
@@ -3411,7 +3411,7 @@
         <v>32</v>
       </c>
       <c r="E191" t="n">
-        <v>0.027899999999999994</v>
+        <v>-0.0889</v>
       </c>
     </row>
     <row r="192">
@@ -3428,7 +3428,7 @@
         <v>32</v>
       </c>
       <c r="E192" t="n">
-        <v>0.027800000000000005</v>
+        <v>-0.08880000000000002</v>
       </c>
     </row>
     <row r="193">
@@ -3445,7 +3445,7 @@
         <v>32</v>
       </c>
       <c r="E193" t="n">
-        <v>-0.0238</v>
+        <v>-0.03720000000000001</v>
       </c>
     </row>
     <row r="194">
@@ -3462,7 +3462,7 @@
         <v>32</v>
       </c>
       <c r="E194" t="n">
-        <v>0.011249999999999996</v>
+        <v>-0.10475</v>
       </c>
     </row>
     <row r="195">
@@ -3479,7 +3479,7 @@
         <v>32</v>
       </c>
       <c r="E195" t="n">
-        <v>-0.01004999999999999</v>
+        <v>-0.08345000000000001</v>
       </c>
     </row>
     <row r="196">
@@ -3496,7 +3496,7 @@
         <v>32</v>
       </c>
       <c r="E196" t="n">
-        <v>-0.02314999999999999</v>
+        <v>-0.07035000000000001</v>
       </c>
     </row>
     <row r="197">
@@ -3513,7 +3513,7 @@
         <v>32</v>
       </c>
       <c r="E197" t="n">
-        <v>4.5000000000000595E-4</v>
+        <v>-0.09395</v>
       </c>
     </row>
     <row r="198">
@@ -3530,7 +3530,7 @@
         <v>32</v>
       </c>
       <c r="E198" t="n">
-        <v>0.029250000000000012</v>
+        <v>-0.12275000000000001</v>
       </c>
     </row>
     <row r="199">
@@ -3547,7 +3547,7 @@
         <v>32</v>
       </c>
       <c r="E199" t="n">
-        <v>0.004250000000000018</v>
+        <v>-0.09775000000000002</v>
       </c>
     </row>
     <row r="200">
@@ -3564,7 +3564,7 @@
         <v>32</v>
       </c>
       <c r="E200" t="n">
-        <v>-0.015750000000000014</v>
+        <v>0.047849999999999976</v>
       </c>
     </row>
     <row r="201">
@@ -3581,7 +3581,7 @@
         <v>32</v>
       </c>
       <c r="E201" t="n">
-        <v>-0.005850000000000008</v>
+        <v>0.03794999999999997</v>
       </c>
     </row>
     <row r="202">
@@ -3598,7 +3598,7 @@
         <v>32</v>
       </c>
       <c r="E202" t="n">
-        <v>-0.012650000000000008</v>
+        <v>0.04474999999999997</v>
       </c>
     </row>
     <row r="203">
@@ -3615,7 +3615,7 @@
         <v>32</v>
       </c>
       <c r="E203" t="n">
-        <v>-0.01945000000000001</v>
+        <v>0.05154999999999997</v>
       </c>
     </row>
     <row r="204">
@@ -3632,7 +3632,7 @@
         <v>32</v>
       </c>
       <c r="E204" t="n">
-        <v>-0.012050000000000005</v>
+        <v>0.04414999999999997</v>
       </c>
     </row>
     <row r="205">
@@ -3649,7 +3649,7 @@
         <v>32</v>
       </c>
       <c r="E205" t="n">
-        <v>-0.021350000000000008</v>
+        <v>0.05344999999999997</v>
       </c>
     </row>
     <row r="206">
@@ -3666,7 +3666,7 @@
         <v>32</v>
       </c>
       <c r="E206" t="n">
-        <v>-1.0000000000000286E-4</v>
+        <v>-0.0752</v>
       </c>
     </row>
     <row r="207">
@@ -3683,7 +3683,7 @@
         <v>32</v>
       </c>
       <c r="E207" t="n">
-        <v>0.007000000000000006</v>
+        <v>-0.08230000000000001</v>
       </c>
     </row>
     <row r="208">
@@ -3700,7 +3700,7 @@
         <v>32</v>
       </c>
       <c r="E208" t="n">
-        <v>-0.004400000000000001</v>
+        <v>-0.0709</v>
       </c>
     </row>
     <row r="209">
@@ -3717,7 +3717,7 @@
         <v>32</v>
       </c>
       <c r="E209" t="n">
-        <v>-0.013700000000000004</v>
+        <v>-0.0616</v>
       </c>
     </row>
     <row r="210">
@@ -3734,7 +3734,7 @@
         <v>32</v>
       </c>
       <c r="E210" t="n">
-        <v>-3.999999999999976E-4</v>
+        <v>-0.07490000000000001</v>
       </c>
     </row>
     <row r="211">
@@ -3751,7 +3751,7 @@
         <v>32</v>
       </c>
       <c r="E211" t="n">
-        <v>-0.020500000000000004</v>
+        <v>-0.0548</v>
       </c>
     </row>
     <row r="212">
@@ -3768,7 +3768,7 @@
         <v>32</v>
       </c>
       <c r="E212" t="n">
-        <v>0.0121</v>
+        <v>-0.05009999999999999</v>
       </c>
     </row>
     <row r="213">
@@ -3785,7 +3785,7 @@
         <v>32</v>
       </c>
       <c r="E213" t="n">
-        <v>-0.013600000000000001</v>
+        <v>-0.02439999999999999</v>
       </c>
     </row>
     <row r="214">
@@ -3802,7 +3802,7 @@
         <v>32</v>
       </c>
       <c r="E214" t="n">
-        <v>-0.0133</v>
+        <v>-0.024699999999999993</v>
       </c>
     </row>
     <row r="215">
@@ -3819,7 +3819,7 @@
         <v>32</v>
       </c>
       <c r="E215" t="n">
-        <v>-0.009300000000000003</v>
+        <v>-0.02869999999999999</v>
       </c>
     </row>
     <row r="216">
@@ -3836,7 +3836,7 @@
         <v>32</v>
       </c>
       <c r="E216" t="n">
-        <v>0.02600000000000001</v>
+        <v>-0.064</v>
       </c>
     </row>
     <row r="217">
@@ -3853,7 +3853,7 @@
         <v>32</v>
       </c>
       <c r="E217" t="n">
-        <v>0.01859999999999999</v>
+        <v>-0.056599999999999984</v>
       </c>
     </row>
     <row r="218">
@@ -3870,7 +3870,7 @@
         <v>33</v>
       </c>
       <c r="E218" t="n">
-        <v>0.24984999999999996</v>
+        <v>-0.30504999999999993</v>
       </c>
     </row>
     <row r="219">
@@ -3887,7 +3887,7 @@
         <v>33</v>
       </c>
       <c r="E219" t="n">
-        <v>0.8566499999999999</v>
+        <v>-0.9118499999999998</v>
       </c>
     </row>
     <row r="220">
@@ -3904,7 +3904,7 @@
         <v>33</v>
       </c>
       <c r="E220" t="n">
-        <v>0.37244999999999995</v>
+        <v>-0.4276499999999999</v>
       </c>
     </row>
     <row r="221">
@@ -3921,7 +3921,7 @@
         <v>33</v>
       </c>
       <c r="E221" t="n">
-        <v>1.13085</v>
+        <v>-1.1860499999999998</v>
       </c>
     </row>
     <row r="222">
@@ -3938,7 +3938,7 @@
         <v>33</v>
       </c>
       <c r="E222" t="n">
-        <v>0.7899499999999999</v>
+        <v>-0.8451499999999998</v>
       </c>
     </row>
     <row r="223">
@@ -3955,7 +3955,7 @@
         <v>33</v>
       </c>
       <c r="E223" t="n">
-        <v>0.58775</v>
+        <v>-0.6429499999999999</v>
       </c>
     </row>
     <row r="224">
@@ -3972,7 +3972,7 @@
         <v>33</v>
       </c>
       <c r="E224" t="n">
-        <v>0.01739999999999997</v>
+        <v>-0.872</v>
       </c>
     </row>
     <row r="225">
@@ -3989,7 +3989,7 @@
         <v>33</v>
       </c>
       <c r="E225" t="n">
-        <v>0.4102000000000001</v>
+        <v>-1.2648000000000001</v>
       </c>
     </row>
     <row r="226">
@@ -4006,7 +4006,7 @@
         <v>33</v>
       </c>
       <c r="E226" t="n">
-        <v>-0.12529999999999997</v>
+        <v>-0.7293000000000001</v>
       </c>
     </row>
     <row r="227">
@@ -4023,7 +4023,7 @@
         <v>33</v>
       </c>
       <c r="E227" t="n">
-        <v>0.0514</v>
+        <v>-0.906</v>
       </c>
     </row>
     <row r="228">
@@ -4040,7 +4040,7 @@
         <v>33</v>
       </c>
       <c r="E228" t="n">
-        <v>-0.0040999999999999925</v>
+        <v>-0.8505</v>
       </c>
     </row>
     <row r="229">
@@ -4057,7 +4057,7 @@
         <v>33</v>
       </c>
       <c r="E229" t="n">
-        <v>0.5258</v>
+        <v>-1.3804</v>
       </c>
     </row>
     <row r="230">
@@ -4074,7 +4074,7 @@
         <v>33</v>
       </c>
       <c r="E230" t="n">
-        <v>0.36040000000000005</v>
+        <v>-0.99585</v>
       </c>
     </row>
     <row r="231">
@@ -4091,7 +4091,7 @@
         <v>33</v>
       </c>
       <c r="E231" t="n">
-        <v>-0.01869999999999994</v>
+        <v>-0.61675</v>
       </c>
     </row>
     <row r="232">
@@ -4108,7 +4108,7 @@
         <v>33</v>
       </c>
       <c r="E232" t="n">
-        <v>0.24639999999999995</v>
+        <v>-0.8818499999999999</v>
       </c>
     </row>
     <row r="233">
@@ -4125,7 +4125,7 @@
         <v>33</v>
       </c>
       <c r="E233" t="n">
-        <v>-0.0595</v>
+        <v>-0.57595</v>
       </c>
     </row>
     <row r="234">
@@ -4142,7 +4142,7 @@
         <v>33</v>
       </c>
       <c r="E234" t="n">
-        <v>-0.10729999999999995</v>
+        <v>-0.52815</v>
       </c>
     </row>
     <row r="235">
@@ -4159,7 +4159,7 @@
         <v>33</v>
       </c>
       <c r="E235" t="n">
-        <v>0.0016999999999999793</v>
+        <v>-0.6371499999999999</v>
       </c>
     </row>
     <row r="236">
@@ -4176,7 +4176,7 @@
         <v>33</v>
       </c>
       <c r="E236" t="n">
-        <v>0.10509999999999997</v>
+        <v>-0.83875</v>
       </c>
     </row>
     <row r="237">
@@ -4193,7 +4193,7 @@
         <v>33</v>
       </c>
       <c r="E237" t="n">
-        <v>0.5724000000000002</v>
+        <v>-1.3060500000000004</v>
       </c>
     </row>
     <row r="238">
@@ -4210,7 +4210,7 @@
         <v>33</v>
       </c>
       <c r="E238" t="n">
-        <v>0.6117000000000001</v>
+        <v>-1.3453500000000003</v>
       </c>
     </row>
     <row r="239">
@@ -4227,7 +4227,7 @@
         <v>33</v>
       </c>
       <c r="E239" t="n">
-        <v>-0.1692</v>
+        <v>-0.56445</v>
       </c>
     </row>
     <row r="240">
@@ -4244,7 +4244,7 @@
         <v>33</v>
       </c>
       <c r="E240" t="n">
-        <v>0.31779999999999997</v>
+        <v>-1.05145</v>
       </c>
     </row>
     <row r="241">
@@ -4261,7 +4261,7 @@
         <v>33</v>
       </c>
       <c r="E241" t="n">
-        <v>-0.0763</v>
+        <v>-0.65735</v>
       </c>
     </row>
     <row r="242">
@@ -4278,7 +4278,7 @@
         <v>33</v>
       </c>
       <c r="E242" t="n">
-        <v>0.3823499999999999</v>
+        <v>-0.37909999999999994</v>
       </c>
     </row>
     <row r="243">
@@ -4295,7 +4295,7 @@
         <v>33</v>
       </c>
       <c r="E243" t="n">
-        <v>0.32264999999999994</v>
+        <v>-0.31939999999999996</v>
       </c>
     </row>
     <row r="244">
@@ -4312,7 +4312,7 @@
         <v>33</v>
       </c>
       <c r="E244" t="n">
-        <v>0.46185000000000004</v>
+        <v>-0.45860000000000006</v>
       </c>
     </row>
     <row r="245">
@@ -4329,7 +4329,7 @@
         <v>33</v>
       </c>
       <c r="E245" t="n">
-        <v>0.2977499999999999</v>
+        <v>-0.29449999999999993</v>
       </c>
     </row>
     <row r="246">
@@ -4346,7 +4346,7 @@
         <v>33</v>
       </c>
       <c r="E246" t="n">
-        <v>0.35155</v>
+        <v>-0.3483</v>
       </c>
     </row>
     <row r="247">
@@ -4363,7 +4363,7 @@
         <v>33</v>
       </c>
       <c r="E247" t="n">
-        <v>0.30775</v>
+        <v>-0.30450000000000005</v>
       </c>
     </row>
     <row r="248">
@@ -4380,7 +4380,7 @@
         <v>33</v>
       </c>
       <c r="E248" t="n">
-        <v>0.16125</v>
+        <v>-0.6465999999999998</v>
       </c>
     </row>
     <row r="249">
@@ -4397,7 +4397,7 @@
         <v>33</v>
       </c>
       <c r="E249" t="n">
-        <v>0.18725000000000003</v>
+        <v>-0.6725999999999999</v>
       </c>
     </row>
     <row r="250">
@@ -4414,7 +4414,7 @@
         <v>33</v>
       </c>
       <c r="E250" t="n">
-        <v>0.1119500000000001</v>
+        <v>-0.5972999999999999</v>
       </c>
     </row>
     <row r="251">
@@ -4431,7 +4431,7 @@
         <v>33</v>
       </c>
       <c r="E251" t="n">
-        <v>-0.26964999999999995</v>
+        <v>-0.21569999999999992</v>
       </c>
     </row>
     <row r="252">
@@ -4448,7 +4448,7 @@
         <v>33</v>
       </c>
       <c r="E252" t="n">
-        <v>0.6836500000000003</v>
+        <v>-1.169</v>
       </c>
     </row>
     <row r="253">
@@ -4465,7 +4465,7 @@
         <v>33</v>
       </c>
       <c r="E253" t="n">
-        <v>0.9863500000000003</v>
+        <v>-1.4717000000000002</v>
       </c>
     </row>
     <row r="254">
@@ -4482,7 +4482,7 @@
         <v>33</v>
       </c>
       <c r="E254" t="n">
-        <v>0.24255000000000002</v>
+        <v>-0.24389999999999998</v>
       </c>
     </row>
     <row r="255">
@@ -4499,7 +4499,7 @@
         <v>33</v>
       </c>
       <c r="E255" t="n">
-        <v>0.25195</v>
+        <v>-0.25329999999999997</v>
       </c>
     </row>
     <row r="256">
@@ -4516,7 +4516,7 @@
         <v>33</v>
       </c>
       <c r="E256" t="n">
-        <v>0.19965000000000008</v>
+        <v>-0.20100000000000004</v>
       </c>
     </row>
     <row r="257">
@@ -4533,7 +4533,7 @@
         <v>33</v>
       </c>
       <c r="E257" t="n">
-        <v>1.4799500000000003</v>
+        <v>-1.4813000000000003</v>
       </c>
     </row>
     <row r="258">
@@ -4550,7 +4550,7 @@
         <v>33</v>
       </c>
       <c r="E258" t="n">
-        <v>-0.02834999999999996</v>
+        <v>0.026999999999999996</v>
       </c>
     </row>
     <row r="259">
@@ -4567,7 +4567,7 @@
         <v>33</v>
       </c>
       <c r="E259" t="n">
-        <v>0.48655000000000004</v>
+        <v>-0.4879</v>
       </c>
     </row>
     <row r="260">
@@ -4584,7 +4584,7 @@
         <v>33</v>
       </c>
       <c r="E260" t="n">
-        <v>0.05985000000000007</v>
+        <v>-0.10535</v>
       </c>
     </row>
     <row r="261">
@@ -4601,7 +4601,7 @@
         <v>33</v>
       </c>
       <c r="E261" t="n">
-        <v>0.2098500000000001</v>
+        <v>-0.25535</v>
       </c>
     </row>
     <row r="262">
@@ -4618,7 +4618,7 @@
         <v>33</v>
       </c>
       <c r="E262" t="n">
-        <v>0.04605000000000001</v>
+        <v>-0.09154999999999994</v>
       </c>
     </row>
     <row r="263">
@@ -4635,7 +4635,7 @@
         <v>33</v>
       </c>
       <c r="E263" t="n">
-        <v>0.6204500000000001</v>
+        <v>-0.66595</v>
       </c>
     </row>
     <row r="264">
@@ -4652,7 +4652,7 @@
         <v>33</v>
       </c>
       <c r="E264" t="n">
-        <v>-0.009250000000000008</v>
+        <v>-0.03624999999999992</v>
       </c>
     </row>
     <row r="265">
@@ -4669,7 +4669,7 @@
         <v>33</v>
       </c>
       <c r="E265" t="n">
-        <v>0.15905000000000002</v>
+        <v>-0.20454999999999995</v>
       </c>
     </row>
     <row r="266">
@@ -4686,7 +4686,7 @@
         <v>33</v>
       </c>
       <c r="E266" t="n">
-        <v>0.59565</v>
+        <v>-0.8694999999999999</v>
       </c>
     </row>
     <row r="267">
@@ -4703,7 +4703,7 @@
         <v>33</v>
       </c>
       <c r="E267" t="n">
-        <v>-0.13535</v>
+        <v>-0.13849999999999993</v>
       </c>
     </row>
     <row r="268">
@@ -4720,7 +4720,7 @@
         <v>33</v>
       </c>
       <c r="E268" t="n">
-        <v>-0.17955</v>
+        <v>-0.09429999999999994</v>
       </c>
     </row>
     <row r="269">
@@ -4737,7 +4737,7 @@
         <v>33</v>
       </c>
       <c r="E269" t="n">
-        <v>0.48374999999999996</v>
+        <v>-0.7575999999999998</v>
       </c>
     </row>
     <row r="270">
@@ -4754,7 +4754,7 @@
         <v>33</v>
       </c>
       <c r="E270" t="n">
-        <v>0.03694999999999998</v>
+        <v>-0.3107999999999999</v>
       </c>
     </row>
     <row r="271">
@@ -4771,7 +4771,7 @@
         <v>33</v>
       </c>
       <c r="E271" t="n">
-        <v>0.003149999999999986</v>
+        <v>-0.2769999999999999</v>
       </c>
     </row>
     <row r="272">
@@ -4788,7 +4788,7 @@
         <v>33</v>
       </c>
       <c r="E272" t="n">
-        <v>-0.31304999999999994</v>
+        <v>0.14575000000000016</v>
       </c>
     </row>
     <row r="273">
@@ -4805,7 +4805,7 @@
         <v>33</v>
       </c>
       <c r="E273" t="n">
-        <v>0.06915000000000016</v>
+        <v>-0.23644999999999994</v>
       </c>
     </row>
     <row r="274">
@@ -4822,7 +4822,7 @@
         <v>33</v>
       </c>
       <c r="E274" t="n">
-        <v>-0.2469499999999999</v>
+        <v>0.07965000000000011</v>
       </c>
     </row>
     <row r="275">
@@ -4839,7 +4839,7 @@
         <v>33</v>
       </c>
       <c r="E275" t="n">
-        <v>0.2824500000000001</v>
+        <v>-0.44974999999999987</v>
       </c>
     </row>
     <row r="276">
@@ -4856,7 +4856,7 @@
         <v>33</v>
       </c>
       <c r="E276" t="n">
-        <v>-0.15474999999999994</v>
+        <v>-0.012549999999999839</v>
       </c>
     </row>
     <row r="277">
@@ -4873,7 +4873,7 @@
         <v>33</v>
       </c>
       <c r="E277" t="n">
-        <v>-0.09614999999999996</v>
+        <v>-0.07114999999999982</v>
       </c>
     </row>
     <row r="278">
@@ -4890,7 +4890,7 @@
         <v>33</v>
       </c>
       <c r="E278" t="n">
-        <v>0.057699999999999974</v>
+        <v>-0.98285</v>
       </c>
     </row>
     <row r="279">
@@ -4907,7 +4907,7 @@
         <v>33</v>
       </c>
       <c r="E279" t="n">
-        <v>-0.4487000000000001</v>
+        <v>-0.47644999999999993</v>
       </c>
     </row>
     <row r="280">
@@ -4924,7 +4924,7 @@
         <v>33</v>
       </c>
       <c r="E280" t="n">
-        <v>-0.6272000000000001</v>
+        <v>-0.29794999999999994</v>
       </c>
     </row>
     <row r="281">
@@ -4941,7 +4941,7 @@
         <v>33</v>
       </c>
       <c r="E281" t="n">
-        <v>-0.6105999999999999</v>
+        <v>-0.3145500000000001</v>
       </c>
     </row>
     <row r="282">
@@ -4958,7 +4958,7 @@
         <v>33</v>
       </c>
       <c r="E282" t="n">
-        <v>-0.4966</v>
+        <v>-0.42855000000000004</v>
       </c>
     </row>
     <row r="283">
@@ -4975,7 +4975,7 @@
         <v>33</v>
       </c>
       <c r="E283" t="n">
-        <v>-0.6359</v>
+        <v>-0.28925</v>
       </c>
     </row>
     <row r="284">
@@ -4992,7 +4992,7 @@
         <v>33</v>
       </c>
       <c r="E284" t="n">
-        <v>-0.14745000000000008</v>
+        <v>0.8648500000000001</v>
       </c>
     </row>
     <row r="285">
@@ -5009,7 +5009,7 @@
         <v>33</v>
       </c>
       <c r="E285" t="n">
-        <v>-0.32985</v>
+        <v>1.04725</v>
       </c>
     </row>
     <row r="286">
@@ -5026,7 +5026,7 @@
         <v>33</v>
       </c>
       <c r="E286" t="n">
-        <v>-0.3759809999999999</v>
+        <v>1.093381</v>
       </c>
     </row>
     <row r="287">
@@ -5043,7 +5043,7 @@
         <v>33</v>
       </c>
       <c r="E287" t="n">
-        <v>0.10505000000000009</v>
+        <v>0.61235</v>
       </c>
     </row>
     <row r="288">
@@ -5060,7 +5060,7 @@
         <v>33</v>
       </c>
       <c r="E288" t="n">
-        <v>0.08014999999999994</v>
+        <v>0.6372500000000001</v>
       </c>
     </row>
     <row r="289">
@@ -5077,7 +5077,7 @@
         <v>33</v>
       </c>
       <c r="E289" t="n">
-        <v>-0.19445</v>
+        <v>0.91185</v>
       </c>
     </row>
     <row r="290">
@@ -5094,7 +5094,7 @@
         <v>34</v>
       </c>
       <c r="E290" t="n">
-        <v>0.37875000000000014</v>
+        <v>-0.7326499999999996</v>
       </c>
     </row>
     <row r="291">
@@ -5111,7 +5111,7 @@
         <v>34</v>
       </c>
       <c r="E291" t="n">
-        <v>0.8579499999999998</v>
+        <v>-1.2118499999999992</v>
       </c>
     </row>
     <row r="292">
@@ -5128,7 +5128,7 @@
         <v>34</v>
       </c>
       <c r="E292" t="n">
-        <v>0.9402499999999998</v>
+        <v>-1.2941499999999992</v>
       </c>
     </row>
     <row r="293">
@@ -5145,7 +5145,7 @@
         <v>34</v>
       </c>
       <c r="E293" t="n">
-        <v>0.09975000000000023</v>
+        <v>-0.45364999999999966</v>
       </c>
     </row>
     <row r="294">
@@ -5162,7 +5162,7 @@
         <v>34</v>
       </c>
       <c r="E294" t="n">
-        <v>-0.33795</v>
+        <v>-0.015949999999999465</v>
       </c>
     </row>
     <row r="295">
@@ -5179,7 +5179,7 @@
         <v>34</v>
       </c>
       <c r="E295" t="n">
-        <v>-0.2750499999999998</v>
+        <v>-0.07884999999999964</v>
       </c>
     </row>
     <row r="296">
@@ -5196,7 +5196,7 @@
         <v>34</v>
       </c>
       <c r="E296" t="n">
-        <v>-0.21550000000000002</v>
+        <v>-1.5407499999999996</v>
       </c>
     </row>
     <row r="297">
@@ -5213,7 +5213,7 @@
         <v>34</v>
       </c>
       <c r="E297" t="n">
-        <v>0.19020000000000015</v>
+        <v>-1.9464499999999998</v>
       </c>
     </row>
     <row r="298">
@@ -5230,7 +5230,7 @@
         <v>34</v>
       </c>
       <c r="E298" t="n">
-        <v>0.10860000000000003</v>
+        <v>-1.8648499999999997</v>
       </c>
     </row>
     <row r="299">
@@ -5247,7 +5247,7 @@
         <v>34</v>
       </c>
       <c r="E299" t="n">
-        <v>1.0204000000000004</v>
+        <v>-2.77665</v>
       </c>
     </row>
     <row r="300">
@@ -5264,7 +5264,7 @@
         <v>34</v>
       </c>
       <c r="E300" t="n">
-        <v>0.8075999999999999</v>
+        <v>-2.5638499999999995</v>
       </c>
     </row>
     <row r="301">
@@ -5281,7 +5281,7 @@
         <v>34</v>
       </c>
       <c r="E301" t="n">
-        <v>0.2795000000000001</v>
+        <v>-2.0357499999999997</v>
       </c>
     </row>
     <row r="302">
@@ -5298,7 +5298,7 @@
         <v>34</v>
       </c>
       <c r="E302" t="n">
-        <v>0.29054999999999975</v>
+        <v>-1.26845</v>
       </c>
     </row>
     <row r="303">
@@ -5315,7 +5315,7 @@
         <v>34</v>
       </c>
       <c r="E303" t="n">
-        <v>0.9645499999999999</v>
+        <v>-1.94245</v>
       </c>
     </row>
     <row r="304">
@@ -5332,7 +5332,7 @@
         <v>34</v>
       </c>
       <c r="E304" t="n">
-        <v>0.72785</v>
+        <v>-1.70575</v>
       </c>
     </row>
     <row r="305">
@@ -5349,7 +5349,7 @@
         <v>34</v>
       </c>
       <c r="E305" t="n">
-        <v>0.6848499999999998</v>
+        <v>-1.66275</v>
       </c>
     </row>
     <row r="306">
@@ -5366,7 +5366,7 @@
         <v>34</v>
       </c>
       <c r="E306" t="n">
-        <v>-0.029950000000000032</v>
+        <v>-0.9479500000000002</v>
       </c>
     </row>
     <row r="307">
@@ -5383,7 +5383,7 @@
         <v>34</v>
       </c>
       <c r="E307" t="n">
-        <v>0.8825499999999998</v>
+        <v>-1.8604500000000002</v>
       </c>
     </row>
     <row r="308">
@@ -5400,7 +5400,7 @@
         <v>34</v>
       </c>
       <c r="E308" t="n">
-        <v>0.031649999999999956</v>
+        <v>-1.181</v>
       </c>
     </row>
     <row r="309">
@@ -5417,7 +5417,7 @@
         <v>34</v>
       </c>
       <c r="E309" t="n">
-        <v>0.18694999999999995</v>
+        <v>-1.3363</v>
       </c>
     </row>
     <row r="310">
@@ -5434,7 +5434,7 @@
         <v>34</v>
       </c>
       <c r="E310" t="n">
-        <v>0.026449999999999863</v>
+        <v>-1.1758</v>
       </c>
     </row>
     <row r="311">
@@ -5451,7 +5451,7 @@
         <v>34</v>
       </c>
       <c r="E311" t="n">
-        <v>-0.10684999999999989</v>
+        <v>-1.0425000000000002</v>
       </c>
     </row>
     <row r="312">
@@ -5468,7 +5468,7 @@
         <v>34</v>
       </c>
       <c r="E312" t="n">
-        <v>0.14684999999999993</v>
+        <v>-1.2962</v>
       </c>
     </row>
     <row r="313">
@@ -5485,7 +5485,7 @@
         <v>34</v>
       </c>
       <c r="E313" t="n">
-        <v>-0.12395</v>
+        <v>-1.0254</v>
       </c>
     </row>
     <row r="314">
@@ -5502,7 +5502,7 @@
         <v>34</v>
       </c>
       <c r="E314" t="n">
-        <v>-0.0889000000000002</v>
+        <v>-1.17545</v>
       </c>
     </row>
     <row r="315">
@@ -5519,7 +5519,7 @@
         <v>34</v>
       </c>
       <c r="E315" t="n">
-        <v>-0.24530000000000007</v>
+        <v>-1.0190500000000002</v>
       </c>
     </row>
     <row r="316">
@@ -5536,7 +5536,7 @@
         <v>34</v>
       </c>
       <c r="E316" t="n">
-        <v>-0.20599999999999996</v>
+        <v>-1.0583500000000003</v>
       </c>
     </row>
     <row r="317">
@@ -5553,7 +5553,7 @@
         <v>34</v>
       </c>
       <c r="E317" t="n">
-        <v>0.026699999999999946</v>
+        <v>-1.2910500000000003</v>
       </c>
     </row>
     <row r="318">
@@ -5570,7 +5570,7 @@
         <v>34</v>
       </c>
       <c r="E318" t="n">
-        <v>0.12670000000000003</v>
+        <v>-1.3910500000000003</v>
       </c>
     </row>
     <row r="319">
@@ -5587,7 +5587,7 @@
         <v>34</v>
       </c>
       <c r="E319" t="n">
-        <v>0.07779999999999987</v>
+        <v>-1.3421500000000002</v>
       </c>
     </row>
     <row r="320">
@@ -5604,7 +5604,7 @@
         <v>34</v>
       </c>
       <c r="E320" t="n">
-        <v>-0.03895000000000004</v>
+        <v>-1.28665</v>
       </c>
     </row>
     <row r="321">
@@ -5621,7 +5621,7 @@
         <v>34</v>
       </c>
       <c r="E321" t="n">
-        <v>0.06994999999999996</v>
+        <v>-1.39555</v>
       </c>
     </row>
     <row r="322">
@@ -5638,7 +5638,7 @@
         <v>34</v>
       </c>
       <c r="E322" t="n">
-        <v>-0.007849999999999913</v>
+        <v>-1.3177500000000002</v>
       </c>
     </row>
     <row r="323">
@@ -5655,7 +5655,7 @@
         <v>34</v>
       </c>
       <c r="E323" t="n">
-        <v>0.29305000000000003</v>
+        <v>-1.6186500000000001</v>
       </c>
     </row>
     <row r="324">
@@ -5672,7 +5672,7 @@
         <v>34</v>
       </c>
       <c r="E324" t="n">
-        <v>0.39005</v>
+        <v>-1.7156500000000001</v>
       </c>
     </row>
     <row r="325">
@@ -5689,7 +5689,7 @@
         <v>34</v>
       </c>
       <c r="E325" t="n">
-        <v>0.24485</v>
+        <v>-1.5704500000000001</v>
       </c>
     </row>
     <row r="326">
@@ -5706,7 +5706,7 @@
         <v>34</v>
       </c>
       <c r="E326" t="n">
-        <v>-0.0017000000000000348</v>
+        <v>-1.2152999999999998</v>
       </c>
     </row>
     <row r="327">
@@ -5723,7 +5723,7 @@
         <v>34</v>
       </c>
       <c r="E327" t="n">
-        <v>-0.11630000000000007</v>
+        <v>-1.1006999999999998</v>
       </c>
     </row>
     <row r="328">
@@ -5740,7 +5740,7 @@
         <v>34</v>
       </c>
       <c r="E328" t="n">
-        <v>-0.07509999999999994</v>
+        <v>-1.1419</v>
       </c>
     </row>
     <row r="329">
@@ -5757,7 +5757,7 @@
         <v>34</v>
       </c>
       <c r="E329" t="n">
-        <v>0.2371000000000001</v>
+        <v>-1.4541</v>
       </c>
     </row>
     <row r="330">
@@ -5774,7 +5774,7 @@
         <v>34</v>
       </c>
       <c r="E330" t="n">
-        <v>-0.12569999999999992</v>
+        <v>-1.0913</v>
       </c>
     </row>
     <row r="331">
@@ -5791,7 +5791,7 @@
         <v>34</v>
       </c>
       <c r="E331" t="n">
-        <v>0.05449999999999999</v>
+        <v>-1.2714999999999999</v>
       </c>
     </row>
     <row r="332">
@@ -5808,7 +5808,7 @@
         <v>34</v>
       </c>
       <c r="E332" t="n">
-        <v>0.42110000000000014</v>
+        <v>-1.1984500000000002</v>
       </c>
     </row>
     <row r="333">
@@ -5825,7 +5825,7 @@
         <v>34</v>
       </c>
       <c r="E333" t="n">
-        <v>0.4611000000000002</v>
+        <v>-1.2384500000000003</v>
       </c>
     </row>
     <row r="334">
@@ -5842,7 +5842,7 @@
         <v>34</v>
       </c>
       <c r="E334" t="n">
-        <v>0.7852</v>
+        <v>-1.5625499999999999</v>
       </c>
     </row>
     <row r="335">
@@ -5859,7 +5859,7 @@
         <v>34</v>
       </c>
       <c r="E335" t="n">
-        <v>0.9856000000000001</v>
+        <v>-1.76295</v>
       </c>
     </row>
     <row r="336">
@@ -5876,7 +5876,7 @@
         <v>34</v>
       </c>
       <c r="E336" t="n">
-        <v>0.5456</v>
+        <v>-1.32295</v>
       </c>
     </row>
     <row r="337">
@@ -5893,7 +5893,7 @@
         <v>34</v>
       </c>
       <c r="E337" t="n">
-        <v>0.33720000000000006</v>
+        <v>-1.11455</v>
       </c>
     </row>
     <row r="338">
@@ -5910,7 +5910,7 @@
         <v>34</v>
       </c>
       <c r="E338" t="n">
-        <v>0.23770000000000002</v>
+        <v>-1.70265</v>
       </c>
     </row>
     <row r="339">
@@ -5927,7 +5927,7 @@
         <v>34</v>
       </c>
       <c r="E339" t="n">
-        <v>2.221</v>
+        <v>-3.68595</v>
       </c>
     </row>
     <row r="340">
@@ -5944,7 +5944,7 @@
         <v>34</v>
       </c>
       <c r="E340" t="n">
-        <v>0.8176999999999999</v>
+        <v>-2.28265</v>
       </c>
     </row>
     <row r="341">
@@ -5961,7 +5961,7 @@
         <v>34</v>
       </c>
       <c r="E341" t="n">
-        <v>0.10150000000000015</v>
+        <v>-1.5664500000000001</v>
       </c>
     </row>
     <row r="342">
@@ -5978,7 +5978,7 @@
         <v>34</v>
       </c>
       <c r="E342" t="n">
-        <v>2.1175</v>
+        <v>-3.58245</v>
       </c>
     </row>
     <row r="343">
@@ -5995,7 +5995,7 @@
         <v>34</v>
       </c>
       <c r="E343" t="n">
-        <v>0.9908999999999999</v>
+        <v>-2.45585</v>
       </c>
     </row>
     <row r="344">
@@ -6012,7 +6012,7 @@
         <v>34</v>
       </c>
       <c r="E344" t="n">
-        <v>-0.6142500000000002</v>
+        <v>-1.5606</v>
       </c>
     </row>
     <row r="345">
@@ -6029,7 +6029,7 @@
         <v>34</v>
       </c>
       <c r="E345" t="n">
-        <v>-1.24085</v>
+        <v>-0.9340000000000002</v>
       </c>
     </row>
     <row r="346">
@@ -6046,7 +6046,7 @@
         <v>34</v>
       </c>
       <c r="E346" t="n">
-        <v>-0.09965000000000002</v>
+        <v>-2.0752</v>
       </c>
     </row>
     <row r="347">
@@ -6063,7 +6063,7 @@
         <v>34</v>
       </c>
       <c r="E347" t="n">
-        <v>-0.3478500000000002</v>
+        <v>-1.827</v>
       </c>
     </row>
     <row r="348">
@@ -6080,7 +6080,7 @@
         <v>34</v>
       </c>
       <c r="E348" t="n">
-        <v>-0.42895000000000016</v>
+        <v>-1.7459</v>
       </c>
     </row>
     <row r="349">
@@ -6097,7 +6097,7 @@
         <v>34</v>
       </c>
       <c r="E349" t="n">
-        <v>-0.5217500000000002</v>
+        <v>-1.6531</v>
       </c>
     </row>
     <row r="350">
@@ -6114,7 +6114,7 @@
         <v>34</v>
       </c>
       <c r="E350" t="n">
-        <v>0.7119000000000004</v>
+        <v>-3.1015</v>
       </c>
     </row>
     <row r="351">
@@ -6131,7 +6131,7 @@
         <v>34</v>
       </c>
       <c r="E351" t="n">
-        <v>-0.9260999999999999</v>
+        <v>-1.4634999999999998</v>
       </c>
     </row>
     <row r="352">
@@ -6148,7 +6148,7 @@
         <v>34</v>
       </c>
       <c r="E352" t="n">
-        <v>-0.9365000000000001</v>
+        <v>-1.4530999999999996</v>
       </c>
     </row>
     <row r="353">
@@ -6165,7 +6165,7 @@
         <v>34</v>
       </c>
       <c r="E353" t="n">
-        <v>-0.5024</v>
+        <v>-1.8871999999999998</v>
       </c>
     </row>
     <row r="354">
@@ -6182,7 +6182,7 @@
         <v>34</v>
       </c>
       <c r="E354" t="n">
-        <v>-0.5952</v>
+        <v>-1.7943999999999998</v>
       </c>
     </row>
     <row r="355">
@@ -6199,7 +6199,7 @@
         <v>34</v>
       </c>
       <c r="E355" t="n">
-        <v>-0.4796</v>
+        <v>-1.9099999999999997</v>
       </c>
     </row>
     <row r="356">
@@ -6216,7 +6216,7 @@
         <v>34</v>
       </c>
       <c r="E356" t="n">
-        <v>-0.48965000000000014</v>
+        <v>-1.17515</v>
       </c>
     </row>
     <row r="357">
@@ -6233,7 +6233,7 @@
         <v>34</v>
       </c>
       <c r="E357" t="n">
-        <v>-0.33614999999999995</v>
+        <v>-1.32865</v>
       </c>
     </row>
     <row r="358">
@@ -6250,7 +6250,7 @@
         <v>34</v>
       </c>
       <c r="E358" t="n">
-        <v>-0.4669500000000002</v>
+        <v>-1.1978499999999999</v>
       </c>
     </row>
     <row r="359">
@@ -6267,7 +6267,7 @@
         <v>34</v>
       </c>
       <c r="E359" t="n">
-        <v>-0.2479499999999999</v>
+        <v>-1.4168500000000002</v>
       </c>
     </row>
     <row r="360">
@@ -6284,7 +6284,7 @@
         <v>34</v>
       </c>
       <c r="E360" t="n">
-        <v>-0.18435</v>
+        <v>-1.48045</v>
       </c>
     </row>
     <row r="361">
@@ -6301,7 +6301,7 @@
         <v>34</v>
       </c>
       <c r="E361" t="n">
-        <v>-0.26675000000000004</v>
+        <v>-1.39805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Functions back to final - initial
</commit_message>
<xml_diff>
--- a/Outputs/Summary/Nutrients_Transplants_data.xlsx
+++ b/Outputs/Summary/Nutrients_Transplants_data.xlsx
@@ -198,7 +198,7 @@
         <v>30</v>
       </c>
       <c r="E2" t="n">
-        <v>-1.9215500000000003</v>
+        <v>0.29345000000000043</v>
       </c>
     </row>
     <row r="3">
@@ -215,7 +215,7 @@
         <v>30</v>
       </c>
       <c r="E3" t="n">
-        <v>-1.49985</v>
+        <v>-0.12824999999999998</v>
       </c>
     </row>
     <row r="4">
@@ -232,7 +232,7 @@
         <v>30</v>
       </c>
       <c r="E4" t="n">
-        <v>-1.4158499999999998</v>
+        <v>-0.21225000000000005</v>
       </c>
     </row>
     <row r="5">
@@ -249,7 +249,7 @@
         <v>30</v>
       </c>
       <c r="E5" t="n">
-        <v>-2.6452500000000003</v>
+        <v>1.0171500000000004</v>
       </c>
     </row>
     <row r="6">
@@ -266,7 +266,7 @@
         <v>30</v>
       </c>
       <c r="E6" t="n">
-        <v>-1.06975</v>
+        <v>-0.5583499999999999</v>
       </c>
     </row>
     <row r="7">
@@ -283,7 +283,7 @@
         <v>30</v>
       </c>
       <c r="E7" t="n">
-        <v>-1.8265500000000001</v>
+        <v>0.19845000000000024</v>
       </c>
     </row>
     <row r="8">
@@ -300,7 +300,7 @@
         <v>30</v>
       </c>
       <c r="E8" t="n">
-        <v>-1.8429499999999999</v>
+        <v>-0.8984500000000002</v>
       </c>
     </row>
     <row r="9">
@@ -317,7 +317,7 @@
         <v>30</v>
       </c>
       <c r="E9" t="n">
-        <v>-2.08835</v>
+        <v>-0.6530500000000001</v>
       </c>
     </row>
     <row r="10">
@@ -334,7 +334,7 @@
         <v>30</v>
       </c>
       <c r="E10" t="n">
-        <v>-1.64505</v>
+        <v>-1.0963500000000002</v>
       </c>
     </row>
     <row r="11">
@@ -351,7 +351,7 @@
         <v>30</v>
       </c>
       <c r="E11" t="n">
-        <v>-2.21715</v>
+        <v>-0.5242500000000001</v>
       </c>
     </row>
     <row r="12">
@@ -368,7 +368,7 @@
         <v>30</v>
       </c>
       <c r="E12" t="n">
-        <v>-2.30115</v>
+        <v>-0.44025000000000003</v>
       </c>
     </row>
     <row r="13">
@@ -385,7 +385,7 @@
         <v>30</v>
       </c>
       <c r="E13" t="n">
-        <v>-3.2848500000000005</v>
+        <v>0.5434500000000002</v>
       </c>
     </row>
     <row r="14">
@@ -402,7 +402,7 @@
         <v>30</v>
       </c>
       <c r="E14" t="n">
-        <v>-4.67065</v>
+        <v>2.24845</v>
       </c>
     </row>
     <row r="15">
@@ -419,7 +419,7 @@
         <v>30</v>
       </c>
       <c r="E15" t="n">
-        <v>-1.8401500000000002</v>
+        <v>-0.58205</v>
       </c>
     </row>
     <row r="16">
@@ -436,7 +436,7 @@
         <v>30</v>
       </c>
       <c r="E16" t="n">
-        <v>-2.2600500000000006</v>
+        <v>-0.1621499999999998</v>
       </c>
     </row>
     <row r="17">
@@ -453,7 +453,7 @@
         <v>30</v>
       </c>
       <c r="E17" t="n">
-        <v>-1.16335</v>
+        <v>-1.25885</v>
       </c>
     </row>
     <row r="18">
@@ -470,7 +470,7 @@
         <v>30</v>
       </c>
       <c r="E18" t="n">
-        <v>-1.16385</v>
+        <v>-1.25835</v>
       </c>
     </row>
     <row r="19">
@@ -487,7 +487,7 @@
         <v>30</v>
       </c>
       <c r="E19" t="n">
-        <v>-1.3462500000000002</v>
+        <v>-1.07595</v>
       </c>
     </row>
     <row r="20">
@@ -504,7 +504,7 @@
         <v>30</v>
       </c>
       <c r="E20" t="n">
-        <v>-6.69665</v>
+        <v>-1.19895</v>
       </c>
     </row>
     <row r="21">
@@ -521,7 +521,7 @@
         <v>30</v>
       </c>
       <c r="E21" t="n">
-        <v>-9.41785</v>
+        <v>1.5222499999999997</v>
       </c>
     </row>
     <row r="22">
@@ -538,7 +538,7 @@
         <v>30</v>
       </c>
       <c r="E22" t="n">
-        <v>-9.309650000000001</v>
+        <v>1.4140500000000005</v>
       </c>
     </row>
     <row r="23">
@@ -555,7 +555,7 @@
         <v>30</v>
       </c>
       <c r="E23" t="n">
-        <v>-5.904450000000001</v>
+        <v>-1.9911499999999998</v>
       </c>
     </row>
     <row r="24">
@@ -572,7 +572,7 @@
         <v>30</v>
       </c>
       <c r="E24" t="n">
-        <v>-8.13315</v>
+        <v>0.2375499999999997</v>
       </c>
     </row>
     <row r="25">
@@ -589,7 +589,7 @@
         <v>30</v>
       </c>
       <c r="E25" t="n">
-        <v>-6.31615</v>
+        <v>-1.57945</v>
       </c>
     </row>
     <row r="26">
@@ -606,7 +606,7 @@
         <v>30</v>
       </c>
       <c r="E26" t="n">
-        <v>-2.9463999999999997</v>
+        <v>-2.3837</v>
       </c>
     </row>
     <row r="27">
@@ -623,7 +623,7 @@
         <v>30</v>
       </c>
       <c r="E27" t="n">
-        <v>-3.4833</v>
+        <v>-1.8468</v>
       </c>
     </row>
     <row r="28">
@@ -640,7 +640,7 @@
         <v>30</v>
       </c>
       <c r="E28" t="n">
-        <v>-3.6980999999999997</v>
+        <v>-1.6320000000000001</v>
       </c>
     </row>
     <row r="29">
@@ -657,7 +657,7 @@
         <v>30</v>
       </c>
       <c r="E29" t="n">
-        <v>-4.5649</v>
+        <v>-0.7652000000000001</v>
       </c>
     </row>
     <row r="30">
@@ -674,7 +674,7 @@
         <v>30</v>
       </c>
       <c r="E30" t="n">
-        <v>-2.9105999999999996</v>
+        <v>-2.4195</v>
       </c>
     </row>
     <row r="31">
@@ -691,7 +691,7 @@
         <v>30</v>
       </c>
       <c r="E31" t="n">
-        <v>-4.4381</v>
+        <v>-0.8919999999999995</v>
       </c>
     </row>
     <row r="32">
@@ -708,7 +708,7 @@
         <v>30</v>
       </c>
       <c r="E32" t="n">
-        <v>-2.2845500000000003</v>
+        <v>-2.47715</v>
       </c>
     </row>
     <row r="33">
@@ -725,7 +725,7 @@
         <v>30</v>
       </c>
       <c r="E33" t="n">
-        <v>-1.85695</v>
+        <v>-2.90475</v>
       </c>
     </row>
     <row r="34">
@@ -742,7 +742,7 @@
         <v>30</v>
       </c>
       <c r="E34" t="n">
-        <v>-1.9756500000000001</v>
+        <v>-2.7860500000000004</v>
       </c>
     </row>
     <row r="35">
@@ -759,7 +759,7 @@
         <v>30</v>
       </c>
       <c r="E35" t="n">
-        <v>-1.76085</v>
+        <v>-3.0008500000000002</v>
       </c>
     </row>
     <row r="36">
@@ -776,7 +776,7 @@
         <v>30</v>
       </c>
       <c r="E36" t="n">
-        <v>-1.85505</v>
+        <v>-2.90665</v>
       </c>
     </row>
     <row r="37">
@@ -793,7 +793,7 @@
         <v>30</v>
       </c>
       <c r="E37" t="n">
-        <v>-2.02735</v>
+        <v>-2.73435</v>
       </c>
     </row>
     <row r="38">
@@ -810,7 +810,7 @@
         <v>30</v>
       </c>
       <c r="E38" t="n">
-        <v>-5.883450000000001</v>
+        <v>-0.8510499999999999</v>
       </c>
     </row>
     <row r="39">
@@ -827,7 +827,7 @@
         <v>30</v>
       </c>
       <c r="E39" t="n">
-        <v>-1.5482500000000008</v>
+        <v>-5.186249999999999</v>
       </c>
     </row>
     <row r="40">
@@ -844,7 +844,7 @@
         <v>30</v>
       </c>
       <c r="E40" t="n">
-        <v>-5.58105</v>
+        <v>-1.1534500000000003</v>
       </c>
     </row>
     <row r="41">
@@ -861,7 +861,7 @@
         <v>30</v>
       </c>
       <c r="E41" t="n">
-        <v>-4.707050000000001</v>
+        <v>-2.02745</v>
       </c>
     </row>
     <row r="42">
@@ -878,7 +878,7 @@
         <v>30</v>
       </c>
       <c r="E42" t="n">
-        <v>-0.48595000000000077</v>
+        <v>-6.24855</v>
       </c>
     </row>
     <row r="43">
@@ -895,7 +895,7 @@
         <v>30</v>
       </c>
       <c r="E43" t="n">
-        <v>-1.8796500000000003</v>
+        <v>-4.854850000000001</v>
       </c>
     </row>
     <row r="44">
@@ -912,7 +912,7 @@
         <v>30</v>
       </c>
       <c r="E44" t="n">
-        <v>-0.3503000000000003</v>
+        <v>-5.0329999999999995</v>
       </c>
     </row>
     <row r="45">
@@ -929,7 +929,7 @@
         <v>30</v>
       </c>
       <c r="E45" t="n">
-        <v>-4.2035</v>
+        <v>-1.1798000000000002</v>
       </c>
     </row>
     <row r="46">
@@ -946,7 +946,7 @@
         <v>30</v>
       </c>
       <c r="E46" t="n">
-        <v>-1.4600000000000004</v>
+        <v>-3.9233</v>
       </c>
     </row>
     <row r="47">
@@ -963,7 +963,7 @@
         <v>30</v>
       </c>
       <c r="E47" t="n">
-        <v>-4.0286</v>
+        <v>-1.3547000000000002</v>
       </c>
     </row>
     <row r="48">
@@ -980,7 +980,7 @@
         <v>30</v>
       </c>
       <c r="E48" t="n">
-        <v>-0.9463000000000004</v>
+        <v>-4.436999999999999</v>
       </c>
     </row>
     <row r="49">
@@ -997,7 +997,7 @@
         <v>30</v>
       </c>
       <c r="E49" t="n">
-        <v>0.02829999999999977</v>
+        <v>-5.4116</v>
       </c>
     </row>
     <row r="50">
@@ -1014,7 +1014,7 @@
         <v>30</v>
       </c>
       <c r="E50" t="n">
-        <v>0.15700000000000047</v>
+        <v>-5.312900000000001</v>
       </c>
     </row>
     <row r="51">
@@ -1031,7 +1031,7 @@
         <v>30</v>
       </c>
       <c r="E51" t="n">
-        <v>0.016300000000000203</v>
+        <v>-5.1722</v>
       </c>
     </row>
     <row r="52">
@@ -1048,7 +1048,7 @@
         <v>30</v>
       </c>
       <c r="E52" t="n">
-        <v>0.9139000000000004</v>
+        <v>-6.069800000000001</v>
       </c>
     </row>
     <row r="53">
@@ -1065,7 +1065,7 @@
         <v>30</v>
       </c>
       <c r="E53" t="n">
-        <v>-2.4012</v>
+        <v>-2.7547</v>
       </c>
     </row>
     <row r="54">
@@ -1082,7 +1082,7 @@
         <v>30</v>
       </c>
       <c r="E54" t="n">
-        <v>-0.46809999999999974</v>
+        <v>-4.6878</v>
       </c>
     </row>
     <row r="55">
@@ -1099,7 +1099,7 @@
         <v>30</v>
       </c>
       <c r="E55" t="n">
-        <v>0.12560000000000038</v>
+        <v>-5.2815</v>
       </c>
     </row>
     <row r="56">
@@ -1116,7 +1116,7 @@
         <v>30</v>
       </c>
       <c r="E56" t="n">
-        <v>-0.19430000000000014</v>
+        <v>-1.6896</v>
       </c>
     </row>
     <row r="57">
@@ -1133,7 +1133,7 @@
         <v>30</v>
       </c>
       <c r="E57" t="n">
-        <v>-0.7570000000000001</v>
+        <v>-1.1269</v>
       </c>
     </row>
     <row r="58">
@@ -1150,7 +1150,7 @@
         <v>30</v>
       </c>
       <c r="E58" t="n">
-        <v>-0.1363000000000002</v>
+        <v>-1.7475999999999998</v>
       </c>
     </row>
     <row r="59">
@@ -1167,7 +1167,7 @@
         <v>30</v>
       </c>
       <c r="E59" t="n">
-        <v>-0.6100000000000002</v>
+        <v>-1.2738999999999998</v>
       </c>
     </row>
     <row r="60">
@@ -1184,7 +1184,7 @@
         <v>30</v>
       </c>
       <c r="E60" t="n">
-        <v>-2.1483000000000003</v>
+        <v>0.2644000000000002</v>
       </c>
     </row>
     <row r="61">
@@ -1201,7 +1201,7 @@
         <v>30</v>
       </c>
       <c r="E61" t="n">
-        <v>-1.2509000000000001</v>
+        <v>-0.633</v>
       </c>
     </row>
     <row r="62">
@@ -1218,7 +1218,7 @@
         <v>30</v>
       </c>
       <c r="E62" t="n">
-        <v>-7.175199999999999</v>
+        <v>2.6408999999999994</v>
       </c>
     </row>
     <row r="63">
@@ -1235,7 +1235,7 @@
         <v>30</v>
       </c>
       <c r="E63" t="n">
-        <v>-2.8874000000000004</v>
+        <v>-1.6468999999999998</v>
       </c>
     </row>
     <row r="64">
@@ -1252,7 +1252,7 @@
         <v>30</v>
       </c>
       <c r="E64" t="n">
-        <v>-1.9024000000000003</v>
+        <v>-2.6319</v>
       </c>
     </row>
     <row r="65">
@@ -1269,7 +1269,7 @@
         <v>30</v>
       </c>
       <c r="E65" t="n">
-        <v>-1.8333000000000004</v>
+        <v>-2.7009999999999996</v>
       </c>
     </row>
     <row r="66">
@@ -1286,7 +1286,7 @@
         <v>30</v>
       </c>
       <c r="E66" t="n">
-        <v>-1.9638000000000002</v>
+        <v>-2.5705</v>
       </c>
     </row>
     <row r="67">
@@ -1303,7 +1303,7 @@
         <v>30</v>
       </c>
       <c r="E67" t="n">
-        <v>-1.5582000000000003</v>
+        <v>-2.9760999999999997</v>
       </c>
     </row>
     <row r="68">
@@ -1320,7 +1320,7 @@
         <v>30</v>
       </c>
       <c r="E68" t="n">
-        <v>0.23665000000000003</v>
+        <v>-3.49645</v>
       </c>
     </row>
     <row r="69">
@@ -1337,7 +1337,7 @@
         <v>30</v>
       </c>
       <c r="E69" t="n">
-        <v>0.2761500000000001</v>
+        <v>-3.5359499999999997</v>
       </c>
     </row>
     <row r="70">
@@ -1354,7 +1354,7 @@
         <v>30</v>
       </c>
       <c r="E70" t="n">
-        <v>0.6569499999999999</v>
+        <v>-3.9167499999999995</v>
       </c>
     </row>
     <row r="71">
@@ -1371,7 +1371,7 @@
         <v>30</v>
       </c>
       <c r="E71" t="n">
-        <v>0.1110500000000001</v>
+        <v>-3.37085</v>
       </c>
     </row>
     <row r="72">
@@ -1388,7 +1388,7 @@
         <v>30</v>
       </c>
       <c r="E72" t="n">
-        <v>-0.5686499999999999</v>
+        <v>-2.69115</v>
       </c>
     </row>
     <row r="73">
@@ -1405,7 +1405,7 @@
         <v>30</v>
       </c>
       <c r="E73" t="n">
-        <v>0.17595000000000005</v>
+        <v>-3.4357499999999996</v>
       </c>
     </row>
     <row r="74">
@@ -1422,7 +1422,7 @@
         <v>31</v>
       </c>
       <c r="E74" t="n">
-        <v>-0.09749999999999999</v>
+        <v>0.022699999999999984</v>
       </c>
     </row>
     <row r="75">
@@ -1439,7 +1439,7 @@
         <v>31</v>
       </c>
       <c r="E75" t="n">
-        <v>-0.0949</v>
+        <v>0.020099999999999993</v>
       </c>
     </row>
     <row r="76">
@@ -1456,7 +1456,7 @@
         <v>31</v>
       </c>
       <c r="E76" t="n">
-        <v>-0.3399</v>
+        <v>0.2651</v>
       </c>
     </row>
     <row r="77">
@@ -1473,7 +1473,7 @@
         <v>31</v>
       </c>
       <c r="E77" t="n">
-        <v>-0.17670000000000002</v>
+        <v>0.1019</v>
       </c>
     </row>
     <row r="78">
@@ -1490,7 +1490,7 @@
         <v>31</v>
       </c>
       <c r="E78" t="n">
-        <v>-0.199</v>
+        <v>0.12419999999999999</v>
       </c>
     </row>
     <row r="79">
@@ -1507,7 +1507,7 @@
         <v>31</v>
       </c>
       <c r="E79" t="n">
-        <v>-0.2444</v>
+        <v>0.16959999999999997</v>
       </c>
     </row>
     <row r="80">
@@ -1524,7 +1524,7 @@
         <v>31</v>
       </c>
       <c r="E80" t="n">
-        <v>-0.20125</v>
+        <v>-0.12344999999999998</v>
       </c>
     </row>
     <row r="81">
@@ -1541,7 +1541,7 @@
         <v>31</v>
       </c>
       <c r="E81" t="n">
-        <v>-0.21895</v>
+        <v>-0.10574999999999998</v>
       </c>
     </row>
     <row r="82">
@@ -1558,7 +1558,7 @@
         <v>31</v>
       </c>
       <c r="E82" t="n">
-        <v>-0.16765000000000002</v>
+        <v>-0.15704999999999997</v>
       </c>
     </row>
     <row r="83">
@@ -1575,7 +1575,7 @@
         <v>31</v>
       </c>
       <c r="E83" t="n">
-        <v>-0.42055</v>
+        <v>0.09584999999999999</v>
       </c>
     </row>
     <row r="84">
@@ -1592,7 +1592,7 @@
         <v>31</v>
       </c>
       <c r="E84" t="n">
-        <v>-0.18775</v>
+        <v>-0.13695</v>
       </c>
     </row>
     <row r="85">
@@ -1609,7 +1609,7 @@
         <v>31</v>
       </c>
       <c r="E85" t="n">
-        <v>-0.26165</v>
+        <v>-0.06305</v>
       </c>
     </row>
     <row r="86">
@@ -1626,7 +1626,7 @@
         <v>31</v>
       </c>
       <c r="E86" t="n">
-        <v>-0.18030000000000002</v>
+        <v>-0.11780000000000002</v>
       </c>
     </row>
     <row r="87">
@@ -1643,7 +1643,7 @@
         <v>31</v>
       </c>
       <c r="E87" t="n">
-        <v>-0.15990000000000001</v>
+        <v>-0.13820000000000002</v>
       </c>
     </row>
     <row r="88">
@@ -1660,7 +1660,7 @@
         <v>31</v>
       </c>
       <c r="E88" t="n">
-        <v>-0.1957</v>
+        <v>-0.10240000000000002</v>
       </c>
     </row>
     <row r="89">
@@ -1677,7 +1677,7 @@
         <v>31</v>
       </c>
       <c r="E89" t="n">
-        <v>-0.128</v>
+        <v>-0.17010000000000003</v>
       </c>
     </row>
     <row r="90">
@@ -1694,7 +1694,7 @@
         <v>31</v>
       </c>
       <c r="E90" t="n">
-        <v>-0.08510000000000001</v>
+        <v>-0.21300000000000002</v>
       </c>
     </row>
     <row r="91">
@@ -1711,7 +1711,7 @@
         <v>31</v>
       </c>
       <c r="E91" t="n">
-        <v>-0.11270000000000001</v>
+        <v>-0.1854</v>
       </c>
     </row>
     <row r="92">
@@ -1728,7 +1728,7 @@
         <v>31</v>
       </c>
       <c r="E92" t="n">
-        <v>-0.43234999999999996</v>
+        <v>0.08715</v>
       </c>
     </row>
     <row r="93">
@@ -1745,7 +1745,7 @@
         <v>31</v>
       </c>
       <c r="E93" t="n">
-        <v>-0.30905</v>
+        <v>-0.03614999999999996</v>
       </c>
     </row>
     <row r="94">
@@ -1762,7 +1762,7 @@
         <v>31</v>
       </c>
       <c r="E94" t="n">
-        <v>-0.7813500000000001</v>
+        <v>0.43615000000000015</v>
       </c>
     </row>
     <row r="95">
@@ -1779,7 +1779,7 @@
         <v>31</v>
       </c>
       <c r="E95" t="n">
-        <v>-0.24774999999999997</v>
+        <v>-0.09744999999999998</v>
       </c>
     </row>
     <row r="96">
@@ -1796,7 +1796,7 @@
         <v>31</v>
       </c>
       <c r="E96" t="n">
-        <v>-0.30045</v>
+        <v>-0.044749999999999956</v>
       </c>
     </row>
     <row r="97">
@@ -1813,7 +1813,7 @@
         <v>31</v>
       </c>
       <c r="E97" t="n">
-        <v>-0.24904999999999997</v>
+        <v>-0.09614999999999999</v>
       </c>
     </row>
     <row r="98">
@@ -1830,7 +1830,7 @@
         <v>31</v>
       </c>
       <c r="E98" t="n">
-        <v>-0.09784999999999999</v>
+        <v>-0.017250000000000015</v>
       </c>
     </row>
     <row r="99">
@@ -1847,7 +1847,7 @@
         <v>31</v>
       </c>
       <c r="E99" t="n">
-        <v>-0.11305</v>
+        <v>-0.00205000000000001</v>
       </c>
     </row>
     <row r="100">
@@ -1864,7 +1864,7 @@
         <v>31</v>
       </c>
       <c r="E100" t="n">
-        <v>-0.11005</v>
+        <v>-0.005050000000000013</v>
       </c>
     </row>
     <row r="101">
@@ -1881,7 +1881,7 @@
         <v>31</v>
       </c>
       <c r="E101" t="n">
-        <v>-0.12455000000000001</v>
+        <v>0.00945</v>
       </c>
     </row>
     <row r="102">
@@ -1898,7 +1898,7 @@
         <v>31</v>
       </c>
       <c r="E102" t="n">
-        <v>-0.09135</v>
+        <v>-0.023750000000000007</v>
       </c>
     </row>
     <row r="103">
@@ -1915,7 +1915,7 @@
         <v>31</v>
       </c>
       <c r="E103" t="n">
-        <v>-0.10765000000000001</v>
+        <v>-0.007449999999999998</v>
       </c>
     </row>
     <row r="104">
@@ -1932,7 +1932,7 @@
         <v>31</v>
       </c>
       <c r="E104" t="n">
-        <v>-0.0852</v>
+        <v>-0.0676</v>
       </c>
     </row>
     <row r="105">
@@ -1949,7 +1949,7 @@
         <v>31</v>
       </c>
       <c r="E105" t="n">
-        <v>-0.0425</v>
+        <v>-0.11029999999999998</v>
       </c>
     </row>
     <row r="106">
@@ -1966,7 +1966,7 @@
         <v>31</v>
       </c>
       <c r="E106" t="n">
-        <v>-0.1142</v>
+        <v>-0.038599999999999995</v>
       </c>
     </row>
     <row r="107">
@@ -1983,7 +1983,7 @@
         <v>31</v>
       </c>
       <c r="E107" t="n">
-        <v>-0.04050000000000001</v>
+        <v>-0.11229999999999998</v>
       </c>
     </row>
     <row r="108">
@@ -2000,7 +2000,7 @@
         <v>31</v>
       </c>
       <c r="E108" t="n">
-        <v>-0.0839</v>
+        <v>-0.06889999999999999</v>
       </c>
     </row>
     <row r="109">
@@ -2017,7 +2017,7 @@
         <v>31</v>
       </c>
       <c r="E109" t="n">
-        <v>-0.1123</v>
+        <v>-0.040499999999999994</v>
       </c>
     </row>
     <row r="110">
@@ -2034,7 +2034,7 @@
         <v>31</v>
       </c>
       <c r="E110" t="n">
-        <v>-0.33085</v>
+        <v>-0.024950000000000055</v>
       </c>
     </row>
     <row r="111">
@@ -2051,7 +2051,7 @@
         <v>31</v>
       </c>
       <c r="E111" t="n">
-        <v>-0.10984999999999999</v>
+        <v>-0.24595</v>
       </c>
     </row>
     <row r="112">
@@ -2068,7 +2068,7 @@
         <v>31</v>
       </c>
       <c r="E112" t="n">
-        <v>-0.15864999999999999</v>
+        <v>-0.19715000000000002</v>
       </c>
     </row>
     <row r="113">
@@ -2085,7 +2085,7 @@
         <v>31</v>
       </c>
       <c r="E113" t="n">
-        <v>-0.35324999999999995</v>
+        <v>-0.0025500000000000245</v>
       </c>
     </row>
     <row r="114">
@@ -2102,7 +2102,7 @@
         <v>31</v>
       </c>
       <c r="E114" t="n">
-        <v>-0.16424999999999998</v>
+        <v>-0.19155000000000003</v>
       </c>
     </row>
     <row r="115">
@@ -2119,7 +2119,7 @@
         <v>31</v>
       </c>
       <c r="E115" t="n">
-        <v>-0.24534999999999998</v>
+        <v>-0.11045000000000002</v>
       </c>
     </row>
     <row r="116">
@@ -2136,7 +2136,7 @@
         <v>31</v>
       </c>
       <c r="E116" t="n">
-        <v>-0.022649999999999976</v>
+        <v>-0.13425</v>
       </c>
     </row>
     <row r="117">
@@ -2153,7 +2153,7 @@
         <v>31</v>
       </c>
       <c r="E117" t="n">
-        <v>-0.03384999999999999</v>
+        <v>-0.12304999999999999</v>
       </c>
     </row>
     <row r="118">
@@ -2170,7 +2170,7 @@
         <v>31</v>
       </c>
       <c r="E118" t="n">
-        <v>-0.07725000000000001</v>
+        <v>-0.07964999999999997</v>
       </c>
     </row>
     <row r="119">
@@ -2187,7 +2187,7 @@
         <v>31</v>
       </c>
       <c r="E119" t="n">
-        <v>-0.03345000000000001</v>
+        <v>-0.12344999999999998</v>
       </c>
     </row>
     <row r="120">
@@ -2204,7 +2204,7 @@
         <v>31</v>
       </c>
       <c r="E120" t="n">
-        <v>-0.10484999999999997</v>
+        <v>-0.05205000000000001</v>
       </c>
     </row>
     <row r="121">
@@ -2221,7 +2221,7 @@
         <v>31</v>
       </c>
       <c r="E121" t="n">
-        <v>0.025450000000000014</v>
+        <v>-0.18235</v>
       </c>
     </row>
     <row r="122">
@@ -2238,7 +2238,7 @@
         <v>31</v>
       </c>
       <c r="E122" t="n">
-        <v>-0.12284999999999999</v>
+        <v>-0.18585</v>
       </c>
     </row>
     <row r="123">
@@ -2255,7 +2255,7 @@
         <v>31</v>
       </c>
       <c r="E123" t="n">
-        <v>-0.26485</v>
+        <v>-0.04385</v>
       </c>
     </row>
     <row r="124">
@@ -2272,7 +2272,7 @@
         <v>31</v>
       </c>
       <c r="E124" t="n">
-        <v>-0.16405</v>
+        <v>-0.14464999999999997</v>
       </c>
     </row>
     <row r="125">
@@ -2289,7 +2289,7 @@
         <v>31</v>
       </c>
       <c r="E125" t="n">
-        <v>-0.12764999999999999</v>
+        <v>-0.18105</v>
       </c>
     </row>
     <row r="126">
@@ -2306,7 +2306,7 @@
         <v>31</v>
       </c>
       <c r="E126" t="n">
-        <v>-0.23015000000000002</v>
+        <v>-0.07854999999999995</v>
       </c>
     </row>
     <row r="127">
@@ -2323,7 +2323,7 @@
         <v>31</v>
       </c>
       <c r="E127" t="n">
-        <v>-0.16804999999999998</v>
+        <v>-0.14065</v>
       </c>
     </row>
     <row r="128">
@@ -2340,7 +2340,7 @@
         <v>31</v>
       </c>
       <c r="E128" t="n">
-        <v>-0.029849999999999974</v>
+        <v>-0.22775</v>
       </c>
     </row>
     <row r="129">
@@ -2357,7 +2357,7 @@
         <v>31</v>
       </c>
       <c r="E129" t="n">
-        <v>-0.07874999999999999</v>
+        <v>-0.17885</v>
       </c>
     </row>
     <row r="130">
@@ -2374,7 +2374,7 @@
         <v>31</v>
       </c>
       <c r="E130" t="n">
-        <v>-0.00644999999999997</v>
+        <v>-0.25115000000000004</v>
       </c>
     </row>
     <row r="131">
@@ -2391,7 +2391,7 @@
         <v>31</v>
       </c>
       <c r="E131" t="n">
-        <v>-0.07585</v>
+        <v>-0.18175</v>
       </c>
     </row>
     <row r="132">
@@ -2408,7 +2408,7 @@
         <v>31</v>
       </c>
       <c r="E132" t="n">
-        <v>-0.03504999999999997</v>
+        <v>-0.22255000000000003</v>
       </c>
     </row>
     <row r="133">
@@ -2425,7 +2425,7 @@
         <v>31</v>
       </c>
       <c r="E133" t="n">
-        <v>-0.02294999999999997</v>
+        <v>-0.23465000000000003</v>
       </c>
     </row>
     <row r="134">
@@ -2442,7 +2442,7 @@
         <v>31</v>
       </c>
       <c r="E134" t="n">
-        <v>-0.1891</v>
+        <v>-0.00449999999999999</v>
       </c>
     </row>
     <row r="135">
@@ -2459,7 +2459,7 @@
         <v>31</v>
       </c>
       <c r="E135" t="n">
-        <v>-0.1986</v>
+        <v>0.005000000000000018</v>
       </c>
     </row>
     <row r="136">
@@ -2476,7 +2476,7 @@
         <v>31</v>
       </c>
       <c r="E136" t="n">
-        <v>-0.127</v>
+        <v>-0.0666</v>
       </c>
     </row>
     <row r="137">
@@ -2493,7 +2493,7 @@
         <v>31</v>
       </c>
       <c r="E137" t="n">
-        <v>-0.08429999999999999</v>
+        <v>-0.10930000000000001</v>
       </c>
     </row>
     <row r="138">
@@ -2510,7 +2510,7 @@
         <v>31</v>
       </c>
       <c r="E138" t="n">
-        <v>-0.18819999999999998</v>
+        <v>-0.005400000000000002</v>
       </c>
     </row>
     <row r="139">
@@ -2527,7 +2527,7 @@
         <v>31</v>
       </c>
       <c r="E139" t="n">
-        <v>-0.08349999999999999</v>
+        <v>-0.1101</v>
       </c>
     </row>
     <row r="140">
@@ -2544,7 +2544,7 @@
         <v>31</v>
       </c>
       <c r="E140" t="n">
-        <v>-0.19725</v>
+        <v>-0.19965000000000002</v>
       </c>
     </row>
     <row r="141">
@@ -2561,7 +2561,7 @@
         <v>31</v>
       </c>
       <c r="E141" t="n">
-        <v>-0.15395000000000003</v>
+        <v>-0.24295</v>
       </c>
     </row>
     <row r="142">
@@ -2578,7 +2578,7 @@
         <v>31</v>
       </c>
       <c r="E142" t="n">
-        <v>-0.16435000000000002</v>
+        <v>-0.23255</v>
       </c>
     </row>
     <row r="143">
@@ -2595,7 +2595,7 @@
         <v>31</v>
       </c>
       <c r="E143" t="n">
-        <v>-0.16495</v>
+        <v>-0.23195000000000002</v>
       </c>
     </row>
     <row r="144">
@@ -2612,7 +2612,7 @@
         <v>31</v>
       </c>
       <c r="E144" t="n">
-        <v>-0.18635000000000002</v>
+        <v>-0.21055000000000001</v>
       </c>
     </row>
     <row r="145">
@@ -2629,7 +2629,7 @@
         <v>31</v>
       </c>
       <c r="E145" t="n">
-        <v>-0.14915</v>
+        <v>-0.24775000000000003</v>
       </c>
     </row>
     <row r="146">
@@ -2646,7 +2646,7 @@
         <v>32</v>
       </c>
       <c r="E146" t="n">
-        <v>-0.08345</v>
+        <v>-0.01915</v>
       </c>
     </row>
     <row r="147">
@@ -2663,7 +2663,7 @@
         <v>32</v>
       </c>
       <c r="E147" t="n">
-        <v>-0.14445000000000002</v>
+        <v>0.04185000000000001</v>
       </c>
     </row>
     <row r="148">
@@ -2680,7 +2680,7 @@
         <v>32</v>
       </c>
       <c r="E148" t="n">
-        <v>-0.11825000000000001</v>
+        <v>0.01565000000000001</v>
       </c>
     </row>
     <row r="149">
@@ -2697,7 +2697,7 @@
         <v>32</v>
       </c>
       <c r="E149" t="n">
-        <v>-0.16675</v>
+        <v>0.06415</v>
       </c>
     </row>
     <row r="150">
@@ -2714,7 +2714,7 @@
         <v>32</v>
       </c>
       <c r="E150" t="n">
-        <v>-0.10085000000000001</v>
+        <v>-0.0017499999999999877</v>
       </c>
     </row>
     <row r="151">
@@ -2731,7 +2731,7 @@
         <v>32</v>
       </c>
       <c r="E151" t="n">
-        <v>-0.11494999999999998</v>
+        <v>0.012349999999999986</v>
       </c>
     </row>
     <row r="152">
@@ -2748,7 +2748,7 @@
         <v>32</v>
       </c>
       <c r="E152" t="n">
-        <v>-0.08949999999999998</v>
+        <v>-0.10410000000000001</v>
       </c>
     </row>
     <row r="153">
@@ -2765,7 +2765,7 @@
         <v>32</v>
       </c>
       <c r="E153" t="n">
-        <v>-0.12829999999999997</v>
+        <v>-0.06530000000000002</v>
       </c>
     </row>
     <row r="154">
@@ -2782,7 +2782,7 @@
         <v>32</v>
       </c>
       <c r="E154" t="n">
-        <v>-0.09919999999999998</v>
+        <v>-0.09440000000000001</v>
       </c>
     </row>
     <row r="155">
@@ -2799,7 +2799,7 @@
         <v>32</v>
       </c>
       <c r="E155" t="n">
-        <v>-0.12189999999999998</v>
+        <v>-0.07170000000000001</v>
       </c>
     </row>
     <row r="156">
@@ -2816,7 +2816,7 @@
         <v>32</v>
       </c>
       <c r="E156" t="n">
-        <v>-0.1033</v>
+        <v>-0.09029999999999999</v>
       </c>
     </row>
     <row r="157">
@@ -2833,7 +2833,7 @@
         <v>32</v>
       </c>
       <c r="E157" t="n">
-        <v>-0.172</v>
+        <v>-0.021600000000000008</v>
       </c>
     </row>
     <row r="158">
@@ -2850,7 +2850,7 @@
         <v>32</v>
       </c>
       <c r="E158" t="n">
-        <v>-0.1508</v>
+        <v>0.017899999999999985</v>
       </c>
     </row>
     <row r="159">
@@ -2867,7 +2867,7 @@
         <v>32</v>
       </c>
       <c r="E159" t="n">
-        <v>-0.11639999999999999</v>
+        <v>-0.0165</v>
       </c>
     </row>
     <row r="160">
@@ -2884,7 +2884,7 @@
         <v>32</v>
       </c>
       <c r="E160" t="n">
-        <v>-0.12329999999999999</v>
+        <v>-0.009599999999999997</v>
       </c>
     </row>
     <row r="161">
@@ -2901,7 +2901,7 @@
         <v>32</v>
       </c>
       <c r="E161" t="n">
-        <v>-0.1027</v>
+        <v>-0.03019999999999999</v>
       </c>
     </row>
     <row r="162">
@@ -2918,7 +2918,7 @@
         <v>32</v>
       </c>
       <c r="E162" t="n">
-        <v>-0.08489999999999999</v>
+        <v>-0.048</v>
       </c>
     </row>
     <row r="163">
@@ -2935,7 +2935,7 @@
         <v>32</v>
       </c>
       <c r="E163" t="n">
-        <v>-0.118</v>
+        <v>-0.014899999999999997</v>
       </c>
     </row>
     <row r="164">
@@ -2952,7 +2952,7 @@
         <v>32</v>
       </c>
       <c r="E164" t="n">
-        <v>-0.18239999999999998</v>
+        <v>-0.04100000000000001</v>
       </c>
     </row>
     <row r="165">
@@ -2969,7 +2969,7 @@
         <v>32</v>
       </c>
       <c r="E165" t="n">
-        <v>-0.20149999999999998</v>
+        <v>-0.021900000000000003</v>
       </c>
     </row>
     <row r="166">
@@ -2986,7 +2986,7 @@
         <v>32</v>
       </c>
       <c r="E166" t="n">
-        <v>-0.21589999999999998</v>
+        <v>-0.007500000000000007</v>
       </c>
     </row>
     <row r="167">
@@ -3003,7 +3003,7 @@
         <v>32</v>
       </c>
       <c r="E167" t="n">
-        <v>-0.12279999999999999</v>
+        <v>-0.1006</v>
       </c>
     </row>
     <row r="168">
@@ -3020,7 +3020,7 @@
         <v>32</v>
       </c>
       <c r="E168" t="n">
-        <v>-0.1765</v>
+        <v>-0.0469</v>
       </c>
     </row>
     <row r="169">
@@ -3037,7 +3037,7 @@
         <v>32</v>
       </c>
       <c r="E169" t="n">
-        <v>-0.1508</v>
+        <v>-0.0726</v>
       </c>
     </row>
     <row r="170">
@@ -3054,7 +3054,7 @@
         <v>32</v>
       </c>
       <c r="E170" t="n">
-        <v>-0.09359999999999999</v>
+        <v>-0.04450000000000001</v>
       </c>
     </row>
     <row r="171">
@@ -3071,7 +3071,7 @@
         <v>32</v>
       </c>
       <c r="E171" t="n">
-        <v>-0.1169</v>
+        <v>-0.021199999999999997</v>
       </c>
     </row>
     <row r="172">
@@ -3088,7 +3088,7 @@
         <v>32</v>
       </c>
       <c r="E172" t="n">
-        <v>-0.1333</v>
+        <v>-0.004799999999999999</v>
       </c>
     </row>
     <row r="173">
@@ -3105,7 +3105,7 @@
         <v>32</v>
       </c>
       <c r="E173" t="n">
-        <v>-0.11030000000000001</v>
+        <v>-0.02779999999999999</v>
       </c>
     </row>
     <row r="174">
@@ -3122,7 +3122,7 @@
         <v>32</v>
       </c>
       <c r="E174" t="n">
-        <v>-0.078</v>
+        <v>-0.0601</v>
       </c>
     </row>
     <row r="175">
@@ -3139,7 +3139,7 @@
         <v>32</v>
       </c>
       <c r="E175" t="n">
-        <v>-0.0947</v>
+        <v>-0.043399999999999994</v>
       </c>
     </row>
     <row r="176">
@@ -3156,7 +3156,7 @@
         <v>32</v>
       </c>
       <c r="E176" t="n">
-        <v>-0.11059999999999999</v>
+        <v>-0.015799999999999995</v>
       </c>
     </row>
     <row r="177">
@@ -3173,7 +3173,7 @@
         <v>32</v>
       </c>
       <c r="E177" t="n">
-        <v>-0.08679999999999999</v>
+        <v>-0.039599999999999996</v>
       </c>
     </row>
     <row r="178">
@@ -3190,7 +3190,7 @@
         <v>32</v>
       </c>
       <c r="E178" t="n">
-        <v>-0.09579999999999998</v>
+        <v>-0.030600000000000002</v>
       </c>
     </row>
     <row r="179">
@@ -3207,7 +3207,7 @@
         <v>32</v>
       </c>
       <c r="E179" t="n">
-        <v>-0.05839999999999999</v>
+        <v>-0.068</v>
       </c>
     </row>
     <row r="180">
@@ -3224,7 +3224,7 @@
         <v>32</v>
       </c>
       <c r="E180" t="n">
-        <v>-0.08019999999999998</v>
+        <v>-0.046200000000000005</v>
       </c>
     </row>
     <row r="181">
@@ -3241,7 +3241,7 @@
         <v>32</v>
       </c>
       <c r="E181" t="n">
-        <v>-0.11019999999999998</v>
+        <v>-0.016200000000000006</v>
       </c>
     </row>
     <row r="182">
@@ -3258,7 +3258,7 @@
         <v>32</v>
       </c>
       <c r="E182" t="n">
-        <v>-0.10975000000000001</v>
+        <v>-0.07595000000000002</v>
       </c>
     </row>
     <row r="183">
@@ -3275,7 +3275,7 @@
         <v>32</v>
       </c>
       <c r="E183" t="n">
-        <v>-0.07345</v>
+        <v>-0.11225000000000003</v>
       </c>
     </row>
     <row r="184">
@@ -3292,7 +3292,7 @@
         <v>32</v>
       </c>
       <c r="E184" t="n">
-        <v>-0.09755</v>
+        <v>-0.08815000000000003</v>
       </c>
     </row>
     <row r="185">
@@ -3309,7 +3309,7 @@
         <v>32</v>
       </c>
       <c r="E185" t="n">
-        <v>-0.12575</v>
+        <v>-0.05995000000000003</v>
       </c>
     </row>
     <row r="186">
@@ -3326,7 +3326,7 @@
         <v>32</v>
       </c>
       <c r="E186" t="n">
-        <v>-0.05825000000000001</v>
+        <v>-0.12745</v>
       </c>
     </row>
     <row r="187">
@@ -3343,7 +3343,7 @@
         <v>32</v>
       </c>
       <c r="E187" t="n">
-        <v>-0.09135000000000001</v>
+        <v>-0.09435000000000002</v>
       </c>
     </row>
     <row r="188">
@@ -3360,7 +3360,7 @@
         <v>32</v>
       </c>
       <c r="E188" t="n">
-        <v>-0.0819</v>
+        <v>-0.09770000000000001</v>
       </c>
     </row>
     <row r="189">
@@ -3377,7 +3377,7 @@
         <v>32</v>
       </c>
       <c r="E189" t="n">
-        <v>-0.11660000000000001</v>
+        <v>-0.063</v>
       </c>
     </row>
     <row r="190">
@@ -3394,7 +3394,7 @@
         <v>32</v>
       </c>
       <c r="E190" t="n">
-        <v>-0.0753</v>
+        <v>-0.1043</v>
       </c>
     </row>
     <row r="191">
@@ -3411,7 +3411,7 @@
         <v>32</v>
       </c>
       <c r="E191" t="n">
-        <v>-0.0889</v>
+        <v>-0.0907</v>
       </c>
     </row>
     <row r="192">
@@ -3428,7 +3428,7 @@
         <v>32</v>
       </c>
       <c r="E192" t="n">
-        <v>-0.08880000000000002</v>
+        <v>-0.09079999999999999</v>
       </c>
     </row>
     <row r="193">
@@ -3445,7 +3445,7 @@
         <v>32</v>
       </c>
       <c r="E193" t="n">
-        <v>-0.03720000000000001</v>
+        <v>-0.1424</v>
       </c>
     </row>
     <row r="194">
@@ -3462,7 +3462,7 @@
         <v>32</v>
       </c>
       <c r="E194" t="n">
-        <v>-0.10475</v>
+        <v>-0.09815</v>
       </c>
     </row>
     <row r="195">
@@ -3479,7 +3479,7 @@
         <v>32</v>
       </c>
       <c r="E195" t="n">
-        <v>-0.08345000000000001</v>
+        <v>-0.11944999999999999</v>
       </c>
     </row>
     <row r="196">
@@ -3496,7 +3496,7 @@
         <v>32</v>
       </c>
       <c r="E196" t="n">
-        <v>-0.07035000000000001</v>
+        <v>-0.13255</v>
       </c>
     </row>
     <row r="197">
@@ -3513,7 +3513,7 @@
         <v>32</v>
       </c>
       <c r="E197" t="n">
-        <v>-0.09395</v>
+        <v>-0.10894999999999999</v>
       </c>
     </row>
     <row r="198">
@@ -3530,7 +3530,7 @@
         <v>32</v>
       </c>
       <c r="E198" t="n">
-        <v>-0.12275000000000001</v>
+        <v>-0.08014999999999999</v>
       </c>
     </row>
     <row r="199">
@@ -3547,7 +3547,7 @@
         <v>32</v>
       </c>
       <c r="E199" t="n">
-        <v>-0.09775000000000002</v>
+        <v>-0.10514999999999998</v>
       </c>
     </row>
     <row r="200">
@@ -3564,7 +3564,7 @@
         <v>32</v>
       </c>
       <c r="E200" t="n">
-        <v>0.047849999999999976</v>
+        <v>-0.17675</v>
       </c>
     </row>
     <row r="201">
@@ -3581,7 +3581,7 @@
         <v>32</v>
       </c>
       <c r="E201" t="n">
-        <v>0.03794999999999997</v>
+        <v>-0.16685</v>
       </c>
     </row>
     <row r="202">
@@ -3598,7 +3598,7 @@
         <v>32</v>
       </c>
       <c r="E202" t="n">
-        <v>0.04474999999999997</v>
+        <v>-0.17364999999999997</v>
       </c>
     </row>
     <row r="203">
@@ -3615,7 +3615,7 @@
         <v>32</v>
       </c>
       <c r="E203" t="n">
-        <v>0.05154999999999997</v>
+        <v>-0.18045</v>
       </c>
     </row>
     <row r="204">
@@ -3632,7 +3632,7 @@
         <v>32</v>
       </c>
       <c r="E204" t="n">
-        <v>0.04414999999999997</v>
+        <v>-0.17304999999999998</v>
       </c>
     </row>
     <row r="205">
@@ -3649,7 +3649,7 @@
         <v>32</v>
       </c>
       <c r="E205" t="n">
-        <v>0.05344999999999997</v>
+        <v>-0.18234999999999998</v>
       </c>
     </row>
     <row r="206">
@@ -3666,7 +3666,7 @@
         <v>32</v>
       </c>
       <c r="E206" t="n">
-        <v>-0.0752</v>
+        <v>-0.0836</v>
       </c>
     </row>
     <row r="207">
@@ -3683,7 +3683,7 @@
         <v>32</v>
       </c>
       <c r="E207" t="n">
-        <v>-0.08230000000000001</v>
+        <v>-0.07649999999999998</v>
       </c>
     </row>
     <row r="208">
@@ -3700,7 +3700,7 @@
         <v>32</v>
       </c>
       <c r="E208" t="n">
-        <v>-0.0709</v>
+        <v>-0.08789999999999999</v>
       </c>
     </row>
     <row r="209">
@@ -3717,7 +3717,7 @@
         <v>32</v>
       </c>
       <c r="E209" t="n">
-        <v>-0.0616</v>
+        <v>-0.0972</v>
       </c>
     </row>
     <row r="210">
@@ -3734,7 +3734,7 @@
         <v>32</v>
       </c>
       <c r="E210" t="n">
-        <v>-0.07490000000000001</v>
+        <v>-0.08389999999999999</v>
       </c>
     </row>
     <row r="211">
@@ -3751,7 +3751,7 @@
         <v>32</v>
       </c>
       <c r="E211" t="n">
-        <v>-0.0548</v>
+        <v>-0.104</v>
       </c>
     </row>
     <row r="212">
@@ -3768,7 +3768,7 @@
         <v>32</v>
       </c>
       <c r="E212" t="n">
-        <v>-0.05009999999999999</v>
+        <v>-0.0621</v>
       </c>
     </row>
     <row r="213">
@@ -3785,7 +3785,7 @@
         <v>32</v>
       </c>
       <c r="E213" t="n">
-        <v>-0.02439999999999999</v>
+        <v>-0.0878</v>
       </c>
     </row>
     <row r="214">
@@ -3802,7 +3802,7 @@
         <v>32</v>
       </c>
       <c r="E214" t="n">
-        <v>-0.024699999999999993</v>
+        <v>-0.0875</v>
       </c>
     </row>
     <row r="215">
@@ -3819,7 +3819,7 @@
         <v>32</v>
       </c>
       <c r="E215" t="n">
-        <v>-0.02869999999999999</v>
+        <v>-0.0835</v>
       </c>
     </row>
     <row r="216">
@@ -3836,7 +3836,7 @@
         <v>32</v>
       </c>
       <c r="E216" t="n">
-        <v>-0.064</v>
+        <v>-0.04819999999999999</v>
       </c>
     </row>
     <row r="217">
@@ -3853,7 +3853,7 @@
         <v>32</v>
       </c>
       <c r="E217" t="n">
-        <v>-0.056599999999999984</v>
+        <v>-0.05560000000000001</v>
       </c>
     </row>
     <row r="218">
@@ -3870,7 +3870,7 @@
         <v>33</v>
       </c>
       <c r="E218" t="n">
-        <v>-0.30504999999999993</v>
+        <v>-0.0918500000000001</v>
       </c>
     </row>
     <row r="219">
@@ -3887,7 +3887,7 @@
         <v>33</v>
       </c>
       <c r="E219" t="n">
-        <v>-0.9118499999999998</v>
+        <v>0.5149499999999998</v>
       </c>
     </row>
     <row r="220">
@@ -3904,7 +3904,7 @@
         <v>33</v>
       </c>
       <c r="E220" t="n">
-        <v>-0.4276499999999999</v>
+        <v>0.03074999999999989</v>
       </c>
     </row>
     <row r="221">
@@ -3921,7 +3921,7 @@
         <v>33</v>
       </c>
       <c r="E221" t="n">
-        <v>-1.1860499999999998</v>
+        <v>0.7891499999999998</v>
       </c>
     </row>
     <row r="222">
@@ -3938,7 +3938,7 @@
         <v>33</v>
       </c>
       <c r="E222" t="n">
-        <v>-0.8451499999999998</v>
+        <v>0.4482499999999998</v>
       </c>
     </row>
     <row r="223">
@@ -3955,7 +3955,7 @@
         <v>33</v>
       </c>
       <c r="E223" t="n">
-        <v>-0.6429499999999999</v>
+        <v>0.24604999999999994</v>
       </c>
     </row>
     <row r="224">
@@ -3972,7 +3972,7 @@
         <v>33</v>
       </c>
       <c r="E224" t="n">
-        <v>-0.872</v>
+        <v>-0.4466</v>
       </c>
     </row>
     <row r="225">
@@ -3989,7 +3989,7 @@
         <v>33</v>
       </c>
       <c r="E225" t="n">
-        <v>-1.2648000000000001</v>
+        <v>-0.05379999999999985</v>
       </c>
     </row>
     <row r="226">
@@ -4006,7 +4006,7 @@
         <v>33</v>
       </c>
       <c r="E226" t="n">
-        <v>-0.7293000000000001</v>
+        <v>-0.5892999999999999</v>
       </c>
     </row>
     <row r="227">
@@ -4023,7 +4023,7 @@
         <v>33</v>
       </c>
       <c r="E227" t="n">
-        <v>-0.906</v>
+        <v>-0.41259999999999997</v>
       </c>
     </row>
     <row r="228">
@@ -4040,7 +4040,7 @@
         <v>33</v>
       </c>
       <c r="E228" t="n">
-        <v>-0.8505</v>
+        <v>-0.46809999999999996</v>
       </c>
     </row>
     <row r="229">
@@ -4057,7 +4057,7 @@
         <v>33</v>
       </c>
       <c r="E229" t="n">
-        <v>-1.3804</v>
+        <v>0.06180000000000008</v>
       </c>
     </row>
     <row r="230">
@@ -4074,7 +4074,7 @@
         <v>33</v>
       </c>
       <c r="E230" t="n">
-        <v>-0.99585</v>
+        <v>0.09625000000000006</v>
       </c>
     </row>
     <row r="231">
@@ -4091,7 +4091,7 @@
         <v>33</v>
       </c>
       <c r="E231" t="n">
-        <v>-0.61675</v>
+        <v>-0.28284999999999993</v>
       </c>
     </row>
     <row r="232">
@@ -4108,7 +4108,7 @@
         <v>33</v>
       </c>
       <c r="E232" t="n">
-        <v>-0.8818499999999999</v>
+        <v>-0.017750000000000044</v>
       </c>
     </row>
     <row r="233">
@@ -4125,7 +4125,7 @@
         <v>33</v>
       </c>
       <c r="E233" t="n">
-        <v>-0.57595</v>
+        <v>-0.32365</v>
       </c>
     </row>
     <row r="234">
@@ -4142,7 +4142,7 @@
         <v>33</v>
       </c>
       <c r="E234" t="n">
-        <v>-0.52815</v>
+        <v>-0.37144999999999995</v>
       </c>
     </row>
     <row r="235">
@@ -4159,7 +4159,7 @@
         <v>33</v>
       </c>
       <c r="E235" t="n">
-        <v>-0.6371499999999999</v>
+        <v>-0.26245</v>
       </c>
     </row>
     <row r="236">
@@ -4176,7 +4176,7 @@
         <v>33</v>
       </c>
       <c r="E236" t="n">
-        <v>-0.83875</v>
+        <v>-0.11225000000000007</v>
       </c>
     </row>
     <row r="237">
@@ -4193,7 +4193,7 @@
         <v>33</v>
       </c>
       <c r="E237" t="n">
-        <v>-1.3060500000000004</v>
+        <v>0.3550500000000002</v>
       </c>
     </row>
     <row r="238">
@@ -4210,7 +4210,7 @@
         <v>33</v>
       </c>
       <c r="E238" t="n">
-        <v>-1.3453500000000003</v>
+        <v>0.3943500000000001</v>
       </c>
     </row>
     <row r="239">
@@ -4227,7 +4227,7 @@
         <v>33</v>
       </c>
       <c r="E239" t="n">
-        <v>-0.56445</v>
+        <v>-0.38655000000000006</v>
       </c>
     </row>
     <row r="240">
@@ -4244,7 +4244,7 @@
         <v>33</v>
       </c>
       <c r="E240" t="n">
-        <v>-1.05145</v>
+        <v>0.10044999999999993</v>
       </c>
     </row>
     <row r="241">
@@ -4261,7 +4261,7 @@
         <v>33</v>
       </c>
       <c r="E241" t="n">
-        <v>-0.65735</v>
+        <v>-0.2936500000000001</v>
       </c>
     </row>
     <row r="242">
@@ -4278,7 +4278,7 @@
         <v>33</v>
       </c>
       <c r="E242" t="n">
-        <v>-0.37909999999999994</v>
+        <v>-0.13180000000000008</v>
       </c>
     </row>
     <row r="243">
@@ -4295,7 +4295,7 @@
         <v>33</v>
       </c>
       <c r="E243" t="n">
-        <v>-0.31939999999999996</v>
+        <v>-0.19150000000000006</v>
       </c>
     </row>
     <row r="244">
@@ -4312,7 +4312,7 @@
         <v>33</v>
       </c>
       <c r="E244" t="n">
-        <v>-0.45860000000000006</v>
+        <v>-0.05229999999999996</v>
       </c>
     </row>
     <row r="245">
@@ -4329,7 +4329,7 @@
         <v>33</v>
       </c>
       <c r="E245" t="n">
-        <v>-0.29449999999999993</v>
+        <v>-0.2164000000000001</v>
       </c>
     </row>
     <row r="246">
@@ -4346,7 +4346,7 @@
         <v>33</v>
       </c>
       <c r="E246" t="n">
-        <v>-0.3483</v>
+        <v>-0.16260000000000002</v>
       </c>
     </row>
     <row r="247">
@@ -4363,7 +4363,7 @@
         <v>33</v>
       </c>
       <c r="E247" t="n">
-        <v>-0.30450000000000005</v>
+        <v>-0.20639999999999997</v>
       </c>
     </row>
     <row r="248">
@@ -4380,7 +4380,7 @@
         <v>33</v>
       </c>
       <c r="E248" t="n">
-        <v>-0.6465999999999998</v>
+        <v>-0.22510000000000002</v>
       </c>
     </row>
     <row r="249">
@@ -4397,7 +4397,7 @@
         <v>33</v>
       </c>
       <c r="E249" t="n">
-        <v>-0.6725999999999999</v>
+        <v>-0.1991</v>
       </c>
     </row>
     <row r="250">
@@ -4414,7 +4414,7 @@
         <v>33</v>
       </c>
       <c r="E250" t="n">
-        <v>-0.5972999999999999</v>
+        <v>-0.2743999999999999</v>
       </c>
     </row>
     <row r="251">
@@ -4431,7 +4431,7 @@
         <v>33</v>
       </c>
       <c r="E251" t="n">
-        <v>-0.21569999999999992</v>
+        <v>-0.656</v>
       </c>
     </row>
     <row r="252">
@@ -4448,7 +4448,7 @@
         <v>33</v>
       </c>
       <c r="E252" t="n">
-        <v>-1.169</v>
+        <v>0.29730000000000023</v>
       </c>
     </row>
     <row r="253">
@@ -4465,7 +4465,7 @@
         <v>33</v>
       </c>
       <c r="E253" t="n">
-        <v>-1.4717000000000002</v>
+        <v>0.6000000000000002</v>
       </c>
     </row>
     <row r="254">
@@ -4482,7 +4482,7 @@
         <v>33</v>
       </c>
       <c r="E254" t="n">
-        <v>-0.24389999999999998</v>
+        <v>-0.18439999999999998</v>
       </c>
     </row>
     <row r="255">
@@ -4499,7 +4499,7 @@
         <v>33</v>
       </c>
       <c r="E255" t="n">
-        <v>-0.25329999999999997</v>
+        <v>-0.17500000000000002</v>
       </c>
     </row>
     <row r="256">
@@ -4516,7 +4516,7 @@
         <v>33</v>
       </c>
       <c r="E256" t="n">
-        <v>-0.20100000000000004</v>
+        <v>-0.22729999999999992</v>
       </c>
     </row>
     <row r="257">
@@ -4533,7 +4533,7 @@
         <v>33</v>
       </c>
       <c r="E257" t="n">
-        <v>-1.4813000000000003</v>
+        <v>1.0530000000000002</v>
       </c>
     </row>
     <row r="258">
@@ -4550,7 +4550,7 @@
         <v>33</v>
       </c>
       <c r="E258" t="n">
-        <v>0.026999999999999996</v>
+        <v>-0.4552999999999999</v>
       </c>
     </row>
     <row r="259">
@@ -4567,7 +4567,7 @@
         <v>33</v>
       </c>
       <c r="E259" t="n">
-        <v>-0.4879</v>
+        <v>0.059600000000000014</v>
       </c>
     </row>
     <row r="260">
@@ -4584,7 +4584,7 @@
         <v>33</v>
       </c>
       <c r="E260" t="n">
-        <v>-0.10535</v>
+        <v>-0.27614999999999995</v>
       </c>
     </row>
     <row r="261">
@@ -4601,7 +4601,7 @@
         <v>33</v>
       </c>
       <c r="E261" t="n">
-        <v>-0.25535</v>
+        <v>-0.12614999999999993</v>
       </c>
     </row>
     <row r="262">
@@ -4618,7 +4618,7 @@
         <v>33</v>
       </c>
       <c r="E262" t="n">
-        <v>-0.09154999999999994</v>
+        <v>-0.28995000000000004</v>
       </c>
     </row>
     <row r="263">
@@ -4635,7 +4635,7 @@
         <v>33</v>
       </c>
       <c r="E263" t="n">
-        <v>-0.66595</v>
+        <v>0.28445000000000004</v>
       </c>
     </row>
     <row r="264">
@@ -4652,7 +4652,7 @@
         <v>33</v>
       </c>
       <c r="E264" t="n">
-        <v>-0.03624999999999992</v>
+        <v>-0.34525000000000006</v>
       </c>
     </row>
     <row r="265">
@@ -4669,7 +4669,7 @@
         <v>33</v>
       </c>
       <c r="E265" t="n">
-        <v>-0.20454999999999995</v>
+        <v>-0.17695</v>
       </c>
     </row>
     <row r="266">
@@ -4686,7 +4686,7 @@
         <v>33</v>
       </c>
       <c r="E266" t="n">
-        <v>-0.8694999999999999</v>
+        <v>0.2773999999999999</v>
       </c>
     </row>
     <row r="267">
@@ -4703,7 +4703,7 @@
         <v>33</v>
       </c>
       <c r="E267" t="n">
-        <v>-0.13849999999999993</v>
+        <v>-0.4536</v>
       </c>
     </row>
     <row r="268">
@@ -4720,7 +4720,7 @@
         <v>33</v>
       </c>
       <c r="E268" t="n">
-        <v>-0.09429999999999994</v>
+        <v>-0.4978</v>
       </c>
     </row>
     <row r="269">
@@ -4737,7 +4737,7 @@
         <v>33</v>
       </c>
       <c r="E269" t="n">
-        <v>-0.7575999999999998</v>
+        <v>0.16549999999999992</v>
       </c>
     </row>
     <row r="270">
@@ -4754,7 +4754,7 @@
         <v>33</v>
       </c>
       <c r="E270" t="n">
-        <v>-0.3107999999999999</v>
+        <v>-0.28130000000000005</v>
       </c>
     </row>
     <row r="271">
@@ -4771,7 +4771,7 @@
         <v>33</v>
       </c>
       <c r="E271" t="n">
-        <v>-0.2769999999999999</v>
+        <v>-0.31510000000000005</v>
       </c>
     </row>
     <row r="272">
@@ -4788,7 +4788,7 @@
         <v>33</v>
       </c>
       <c r="E272" t="n">
-        <v>0.14575000000000016</v>
+        <v>-1.1908500000000002</v>
       </c>
     </row>
     <row r="273">
@@ -4805,7 +4805,7 @@
         <v>33</v>
       </c>
       <c r="E273" t="n">
-        <v>-0.23644999999999994</v>
+        <v>-0.80865</v>
       </c>
     </row>
     <row r="274">
@@ -4822,7 +4822,7 @@
         <v>33</v>
       </c>
       <c r="E274" t="n">
-        <v>0.07965000000000011</v>
+        <v>-1.1247500000000001</v>
       </c>
     </row>
     <row r="275">
@@ -4839,7 +4839,7 @@
         <v>33</v>
       </c>
       <c r="E275" t="n">
-        <v>-0.44974999999999987</v>
+        <v>-0.59535</v>
       </c>
     </row>
     <row r="276">
@@ -4856,7 +4856,7 @@
         <v>33</v>
       </c>
       <c r="E276" t="n">
-        <v>-0.012549999999999839</v>
+        <v>-1.03255</v>
       </c>
     </row>
     <row r="277">
@@ -4873,7 +4873,7 @@
         <v>33</v>
       </c>
       <c r="E277" t="n">
-        <v>-0.07114999999999982</v>
+        <v>-0.9739500000000001</v>
       </c>
     </row>
     <row r="278">
@@ -4890,7 +4890,7 @@
         <v>33</v>
       </c>
       <c r="E278" t="n">
-        <v>-0.98285</v>
+        <v>-0.75935</v>
       </c>
     </row>
     <row r="279">
@@ -4907,7 +4907,7 @@
         <v>33</v>
       </c>
       <c r="E279" t="n">
-        <v>-0.47644999999999993</v>
+        <v>-1.2657500000000002</v>
       </c>
     </row>
     <row r="280">
@@ -4924,7 +4924,7 @@
         <v>33</v>
       </c>
       <c r="E280" t="n">
-        <v>-0.29794999999999994</v>
+        <v>-1.44425</v>
       </c>
     </row>
     <row r="281">
@@ -4941,7 +4941,7 @@
         <v>33</v>
       </c>
       <c r="E281" t="n">
-        <v>-0.3145500000000001</v>
+        <v>-1.4276499999999999</v>
       </c>
     </row>
     <row r="282">
@@ -4958,7 +4958,7 @@
         <v>33</v>
       </c>
       <c r="E282" t="n">
-        <v>-0.42855000000000004</v>
+        <v>-1.31365</v>
       </c>
     </row>
     <row r="283">
@@ -4975,7 +4975,7 @@
         <v>33</v>
       </c>
       <c r="E283" t="n">
-        <v>-0.28925</v>
+        <v>-1.45295</v>
       </c>
     </row>
     <row r="284">
@@ -4992,7 +4992,7 @@
         <v>33</v>
       </c>
       <c r="E284" t="n">
-        <v>0.8648500000000001</v>
+        <v>-1.61715</v>
       </c>
     </row>
     <row r="285">
@@ -5009,7 +5009,7 @@
         <v>33</v>
       </c>
       <c r="E285" t="n">
-        <v>1.04725</v>
+        <v>-1.79955</v>
       </c>
     </row>
     <row r="286">
@@ -5026,7 +5026,7 @@
         <v>33</v>
       </c>
       <c r="E286" t="n">
-        <v>1.093381</v>
+        <v>-1.845681</v>
       </c>
     </row>
     <row r="287">
@@ -5043,7 +5043,7 @@
         <v>33</v>
       </c>
       <c r="E287" t="n">
-        <v>0.61235</v>
+        <v>-1.36465</v>
       </c>
     </row>
     <row r="288">
@@ -5060,7 +5060,7 @@
         <v>33</v>
       </c>
       <c r="E288" t="n">
-        <v>0.6372500000000001</v>
+        <v>-1.38955</v>
       </c>
     </row>
     <row r="289">
@@ -5077,7 +5077,7 @@
         <v>33</v>
       </c>
       <c r="E289" t="n">
-        <v>0.91185</v>
+        <v>-1.66415</v>
       </c>
     </row>
     <row r="290">
@@ -5094,7 +5094,7 @@
         <v>34</v>
       </c>
       <c r="E290" t="n">
-        <v>-0.7326499999999996</v>
+        <v>-2.2628500000000003</v>
       </c>
     </row>
     <row r="291">
@@ -5111,7 +5111,7 @@
         <v>34</v>
       </c>
       <c r="E291" t="n">
-        <v>-1.2118499999999992</v>
+        <v>-1.7836500000000006</v>
       </c>
     </row>
     <row r="292">
@@ -5128,7 +5128,7 @@
         <v>34</v>
       </c>
       <c r="E292" t="n">
-        <v>-1.2941499999999992</v>
+        <v>-1.7013500000000006</v>
       </c>
     </row>
     <row r="293">
@@ -5145,7 +5145,7 @@
         <v>34</v>
       </c>
       <c r="E293" t="n">
-        <v>-0.45364999999999966</v>
+        <v>-2.54185</v>
       </c>
     </row>
     <row r="294">
@@ -5162,7 +5162,7 @@
         <v>34</v>
       </c>
       <c r="E294" t="n">
-        <v>-0.015949999999999465</v>
+        <v>-2.9795500000000006</v>
       </c>
     </row>
     <row r="295">
@@ -5179,7 +5179,7 @@
         <v>34</v>
       </c>
       <c r="E295" t="n">
-        <v>-0.07884999999999964</v>
+        <v>-2.91665</v>
       </c>
     </row>
     <row r="296">
@@ -5196,7 +5196,7 @@
         <v>34</v>
       </c>
       <c r="E296" t="n">
-        <v>-1.5407499999999996</v>
+        <v>-1.51425</v>
       </c>
     </row>
     <row r="297">
@@ -5213,7 +5213,7 @@
         <v>34</v>
       </c>
       <c r="E297" t="n">
-        <v>-1.9464499999999998</v>
+        <v>-1.10855</v>
       </c>
     </row>
     <row r="298">
@@ -5230,7 +5230,7 @@
         <v>34</v>
       </c>
       <c r="E298" t="n">
-        <v>-1.8648499999999997</v>
+        <v>-1.19015</v>
       </c>
     </row>
     <row r="299">
@@ -5247,7 +5247,7 @@
         <v>34</v>
       </c>
       <c r="E299" t="n">
-        <v>-2.77665</v>
+        <v>-0.27834999999999965</v>
       </c>
     </row>
     <row r="300">
@@ -5264,7 +5264,7 @@
         <v>34</v>
       </c>
       <c r="E300" t="n">
-        <v>-2.5638499999999995</v>
+        <v>-0.4911500000000002</v>
       </c>
     </row>
     <row r="301">
@@ -5281,7 +5281,7 @@
         <v>34</v>
       </c>
       <c r="E301" t="n">
-        <v>-2.0357499999999997</v>
+        <v>-1.01925</v>
       </c>
     </row>
     <row r="302">
@@ -5298,7 +5298,7 @@
         <v>34</v>
       </c>
       <c r="E302" t="n">
-        <v>-1.26845</v>
+        <v>-0.6818500000000002</v>
       </c>
     </row>
     <row r="303">
@@ -5315,7 +5315,7 @@
         <v>34</v>
       </c>
       <c r="E303" t="n">
-        <v>-1.94245</v>
+        <v>-0.007850000000000024</v>
       </c>
     </row>
     <row r="304">
@@ -5332,7 +5332,7 @@
         <v>34</v>
       </c>
       <c r="E304" t="n">
-        <v>-1.70575</v>
+        <v>-0.24454999999999993</v>
       </c>
     </row>
     <row r="305">
@@ -5349,7 +5349,7 @@
         <v>34</v>
       </c>
       <c r="E305" t="n">
-        <v>-1.66275</v>
+        <v>-0.2875500000000001</v>
       </c>
     </row>
     <row r="306">
@@ -5366,7 +5366,7 @@
         <v>34</v>
       </c>
       <c r="E306" t="n">
-        <v>-0.9479500000000002</v>
+        <v>-1.0023499999999999</v>
       </c>
     </row>
     <row r="307">
@@ -5383,7 +5383,7 @@
         <v>34</v>
       </c>
       <c r="E307" t="n">
-        <v>-1.8604500000000002</v>
+        <v>-0.0898500000000001</v>
       </c>
     </row>
     <row r="308">
@@ -5400,7 +5400,7 @@
         <v>34</v>
       </c>
       <c r="E308" t="n">
-        <v>-1.181</v>
+        <v>-1.3489</v>
       </c>
     </row>
     <row r="309">
@@ -5417,7 +5417,7 @@
         <v>34</v>
       </c>
       <c r="E309" t="n">
-        <v>-1.3363</v>
+        <v>-1.1936</v>
       </c>
     </row>
     <row r="310">
@@ -5434,7 +5434,7 @@
         <v>34</v>
       </c>
       <c r="E310" t="n">
-        <v>-1.1758</v>
+        <v>-1.3541</v>
       </c>
     </row>
     <row r="311">
@@ -5451,7 +5451,7 @@
         <v>34</v>
       </c>
       <c r="E311" t="n">
-        <v>-1.0425000000000002</v>
+        <v>-1.4873999999999998</v>
       </c>
     </row>
     <row r="312">
@@ -5468,7 +5468,7 @@
         <v>34</v>
       </c>
       <c r="E312" t="n">
-        <v>-1.2962</v>
+        <v>-1.2337</v>
       </c>
     </row>
     <row r="313">
@@ -5485,7 +5485,7 @@
         <v>34</v>
       </c>
       <c r="E313" t="n">
-        <v>-1.0254</v>
+        <v>-1.5045</v>
       </c>
     </row>
     <row r="314">
@@ -5502,7 +5502,7 @@
         <v>34</v>
       </c>
       <c r="E314" t="n">
-        <v>-1.17545</v>
+        <v>-1.41555</v>
       </c>
     </row>
     <row r="315">
@@ -5519,7 +5519,7 @@
         <v>34</v>
       </c>
       <c r="E315" t="n">
-        <v>-1.0190500000000002</v>
+        <v>-1.57195</v>
       </c>
     </row>
     <row r="316">
@@ -5536,7 +5536,7 @@
         <v>34</v>
       </c>
       <c r="E316" t="n">
-        <v>-1.0583500000000003</v>
+        <v>-1.5326499999999998</v>
       </c>
     </row>
     <row r="317">
@@ -5553,7 +5553,7 @@
         <v>34</v>
       </c>
       <c r="E317" t="n">
-        <v>-1.2910500000000003</v>
+        <v>-1.29995</v>
       </c>
     </row>
     <row r="318">
@@ -5570,7 +5570,7 @@
         <v>34</v>
       </c>
       <c r="E318" t="n">
-        <v>-1.3910500000000003</v>
+        <v>-1.1999499999999999</v>
       </c>
     </row>
     <row r="319">
@@ -5587,7 +5587,7 @@
         <v>34</v>
       </c>
       <c r="E319" t="n">
-        <v>-1.3421500000000002</v>
+        <v>-1.24885</v>
       </c>
     </row>
     <row r="320">
@@ -5604,7 +5604,7 @@
         <v>34</v>
       </c>
       <c r="E320" t="n">
-        <v>-1.28665</v>
+        <v>-1.19105</v>
       </c>
     </row>
     <row r="321">
@@ -5621,7 +5621,7 @@
         <v>34</v>
       </c>
       <c r="E321" t="n">
-        <v>-1.39555</v>
+        <v>-1.08215</v>
       </c>
     </row>
     <row r="322">
@@ -5638,7 +5638,7 @@
         <v>34</v>
       </c>
       <c r="E322" t="n">
-        <v>-1.3177500000000002</v>
+        <v>-1.1599499999999998</v>
       </c>
     </row>
     <row r="323">
@@ -5655,7 +5655,7 @@
         <v>34</v>
       </c>
       <c r="E323" t="n">
-        <v>-1.6186500000000001</v>
+        <v>-0.8590499999999999</v>
       </c>
     </row>
     <row r="324">
@@ -5672,7 +5672,7 @@
         <v>34</v>
       </c>
       <c r="E324" t="n">
-        <v>-1.7156500000000001</v>
+        <v>-0.7620499999999999</v>
       </c>
     </row>
     <row r="325">
@@ -5689,7 +5689,7 @@
         <v>34</v>
       </c>
       <c r="E325" t="n">
-        <v>-1.5704500000000001</v>
+        <v>-0.9072499999999999</v>
       </c>
     </row>
     <row r="326">
@@ -5706,7 +5706,7 @@
         <v>34</v>
       </c>
       <c r="E326" t="n">
-        <v>-1.2152999999999998</v>
+        <v>-1.2049</v>
       </c>
     </row>
     <row r="327">
@@ -5723,7 +5723,7 @@
         <v>34</v>
       </c>
       <c r="E327" t="n">
-        <v>-1.1006999999999998</v>
+        <v>-1.3195000000000001</v>
       </c>
     </row>
     <row r="328">
@@ -5740,7 +5740,7 @@
         <v>34</v>
       </c>
       <c r="E328" t="n">
-        <v>-1.1419</v>
+        <v>-1.2783</v>
       </c>
     </row>
     <row r="329">
@@ -5757,7 +5757,7 @@
         <v>34</v>
       </c>
       <c r="E329" t="n">
-        <v>-1.4541</v>
+        <v>-0.9661</v>
       </c>
     </row>
     <row r="330">
@@ -5774,7 +5774,7 @@
         <v>34</v>
       </c>
       <c r="E330" t="n">
-        <v>-1.0913</v>
+        <v>-1.3289</v>
       </c>
     </row>
     <row r="331">
@@ -5791,7 +5791,7 @@
         <v>34</v>
       </c>
       <c r="E331" t="n">
-        <v>-1.2714999999999999</v>
+        <v>-1.1487</v>
       </c>
     </row>
     <row r="332">
@@ -5808,7 +5808,7 @@
         <v>34</v>
       </c>
       <c r="E332" t="n">
-        <v>-1.1984500000000002</v>
+        <v>-0.6029499999999998</v>
       </c>
     </row>
     <row r="333">
@@ -5825,7 +5825,7 @@
         <v>34</v>
       </c>
       <c r="E333" t="n">
-        <v>-1.2384500000000003</v>
+        <v>-0.5629499999999997</v>
       </c>
     </row>
     <row r="334">
@@ -5842,7 +5842,7 @@
         <v>34</v>
       </c>
       <c r="E334" t="n">
-        <v>-1.5625499999999999</v>
+        <v>-0.2388499999999999</v>
       </c>
     </row>
     <row r="335">
@@ -5859,7 +5859,7 @@
         <v>34</v>
       </c>
       <c r="E335" t="n">
-        <v>-1.76295</v>
+        <v>-0.03844999999999976</v>
       </c>
     </row>
     <row r="336">
@@ -5876,7 +5876,7 @@
         <v>34</v>
       </c>
       <c r="E336" t="n">
-        <v>-1.32295</v>
+        <v>-0.47844999999999993</v>
       </c>
     </row>
     <row r="337">
@@ -5893,7 +5893,7 @@
         <v>34</v>
       </c>
       <c r="E337" t="n">
-        <v>-1.11455</v>
+        <v>-0.6868499999999998</v>
       </c>
     </row>
     <row r="338">
@@ -5910,7 +5910,7 @@
         <v>34</v>
       </c>
       <c r="E338" t="n">
-        <v>-1.70265</v>
+        <v>-1.2867499999999998</v>
       </c>
     </row>
     <row r="339">
@@ -5927,7 +5927,7 @@
         <v>34</v>
       </c>
       <c r="E339" t="n">
-        <v>-3.68595</v>
+        <v>0.6965500000000002</v>
       </c>
     </row>
     <row r="340">
@@ -5944,7 +5944,7 @@
         <v>34</v>
       </c>
       <c r="E340" t="n">
-        <v>-2.28265</v>
+        <v>-0.70675</v>
       </c>
     </row>
     <row r="341">
@@ -5961,7 +5961,7 @@
         <v>34</v>
       </c>
       <c r="E341" t="n">
-        <v>-1.5664500000000001</v>
+        <v>-1.4229499999999997</v>
       </c>
     </row>
     <row r="342">
@@ -5978,7 +5978,7 @@
         <v>34</v>
       </c>
       <c r="E342" t="n">
-        <v>-3.58245</v>
+        <v>0.5930500000000003</v>
       </c>
     </row>
     <row r="343">
@@ -5995,7 +5995,7 @@
         <v>34</v>
       </c>
       <c r="E343" t="n">
-        <v>-2.45585</v>
+        <v>-0.53355</v>
       </c>
     </row>
     <row r="344">
@@ -6012,7 +6012,7 @@
         <v>34</v>
       </c>
       <c r="E344" t="n">
-        <v>-1.5606</v>
+        <v>-2.5273000000000003</v>
       </c>
     </row>
     <row r="345">
@@ -6029,7 +6029,7 @@
         <v>34</v>
       </c>
       <c r="E345" t="n">
-        <v>-0.9340000000000002</v>
+        <v>-3.1539</v>
       </c>
     </row>
     <row r="346">
@@ -6046,7 +6046,7 @@
         <v>34</v>
       </c>
       <c r="E346" t="n">
-        <v>-2.0752</v>
+        <v>-2.0127</v>
       </c>
     </row>
     <row r="347">
@@ -6063,7 +6063,7 @@
         <v>34</v>
       </c>
       <c r="E347" t="n">
-        <v>-1.827</v>
+        <v>-2.2609000000000004</v>
       </c>
     </row>
     <row r="348">
@@ -6080,7 +6080,7 @@
         <v>34</v>
       </c>
       <c r="E348" t="n">
-        <v>-1.7459</v>
+        <v>-2.3420000000000005</v>
       </c>
     </row>
     <row r="349">
@@ -6097,7 +6097,7 @@
         <v>34</v>
       </c>
       <c r="E349" t="n">
-        <v>-1.6531</v>
+        <v>-2.4348</v>
       </c>
     </row>
     <row r="350">
@@ -6114,7 +6114,7 @@
         <v>34</v>
       </c>
       <c r="E350" t="n">
-        <v>-3.1015</v>
+        <v>-1.3577</v>
       </c>
     </row>
     <row r="351">
@@ -6131,7 +6131,7 @@
         <v>34</v>
       </c>
       <c r="E351" t="n">
-        <v>-1.4634999999999998</v>
+        <v>-2.9957000000000003</v>
       </c>
     </row>
     <row r="352">
@@ -6148,7 +6148,7 @@
         <v>34</v>
       </c>
       <c r="E352" t="n">
-        <v>-1.4530999999999996</v>
+        <v>-3.0061000000000004</v>
       </c>
     </row>
     <row r="353">
@@ -6165,7 +6165,7 @@
         <v>34</v>
       </c>
       <c r="E353" t="n">
-        <v>-1.8871999999999998</v>
+        <v>-2.572</v>
       </c>
     </row>
     <row r="354">
@@ -6182,7 +6182,7 @@
         <v>34</v>
       </c>
       <c r="E354" t="n">
-        <v>-1.7943999999999998</v>
+        <v>-2.6648000000000005</v>
       </c>
     </row>
     <row r="355">
@@ -6199,7 +6199,7 @@
         <v>34</v>
       </c>
       <c r="E355" t="n">
-        <v>-1.9099999999999997</v>
+        <v>-2.5492000000000004</v>
       </c>
     </row>
     <row r="356">
@@ -6216,7 +6216,7 @@
         <v>34</v>
       </c>
       <c r="E356" t="n">
-        <v>-1.17515</v>
+        <v>-1.9665500000000002</v>
       </c>
     </row>
     <row r="357">
@@ -6233,7 +6233,7 @@
         <v>34</v>
       </c>
       <c r="E357" t="n">
-        <v>-1.32865</v>
+        <v>-1.81305</v>
       </c>
     </row>
     <row r="358">
@@ -6250,7 +6250,7 @@
         <v>34</v>
       </c>
       <c r="E358" t="n">
-        <v>-1.1978499999999999</v>
+        <v>-1.9438500000000003</v>
       </c>
     </row>
     <row r="359">
@@ -6267,7 +6267,7 @@
         <v>34</v>
       </c>
       <c r="E359" t="n">
-        <v>-1.4168500000000002</v>
+        <v>-1.72485</v>
       </c>
     </row>
     <row r="360">
@@ -6284,7 +6284,7 @@
         <v>34</v>
       </c>
       <c r="E360" t="n">
-        <v>-1.48045</v>
+        <v>-1.6612500000000001</v>
       </c>
     </row>
     <row r="361">
@@ -6301,7 +6301,7 @@
         <v>34</v>
       </c>
       <c r="E361" t="n">
-        <v>-1.39805</v>
+        <v>-1.7436500000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>